<commit_message>
Add deleted paths to Homepage-0 sheet
</commit_message>
<xml_diff>
--- a/Redesign-Redirects.xlsx
+++ b/Redesign-Redirects.xlsx
@@ -8,25 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sampanda/Samshub/test-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ADD9627-B68B-A644-A881-33CEADCC84ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55C7BE8A-F5FA-314F-B250-76ADB85259C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12340" yWindow="3220" windowWidth="32260" windowHeight="23640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Homepage-1" sheetId="2" r:id="rId1"/>
-    <sheet name="Homepage-2" sheetId="3" r:id="rId2"/>
-    <sheet name="Homepage-3" sheetId="4" r:id="rId3"/>
-    <sheet name="Homepage-4" sheetId="5" r:id="rId4"/>
-    <sheet name="Homepage-5" sheetId="6" r:id="rId5"/>
-    <sheet name="Homepage-6" sheetId="7" r:id="rId6"/>
-    <sheet name="JNJ OUR COMPANYPRODUCT URL CLEA" sheetId="1" r:id="rId7"/>
+    <sheet name="Homepage-0" sheetId="8" r:id="rId1"/>
+    <sheet name="Homepage-1" sheetId="2" r:id="rId2"/>
+    <sheet name="Homepage-2" sheetId="3" r:id="rId3"/>
+    <sheet name="Homepage-3" sheetId="4" r:id="rId4"/>
+    <sheet name="Homepage-4" sheetId="5" r:id="rId5"/>
+    <sheet name="Homepage-5" sheetId="6" r:id="rId6"/>
+    <sheet name="Homepage-6" sheetId="7" r:id="rId7"/>
+    <sheet name="JNJ OUR COMPANYPRODUCT URL CLEA" sheetId="1" r:id="rId8"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7083" uniqueCount="2442">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7105" uniqueCount="2464">
   <si>
     <t xml:space="preserve">Name of article </t>
   </si>
@@ -7463,6 +7464,72 @@
   </si>
   <si>
     <t>https://www.jnj.com/2011/10/drive-safely-work-week-and-btw-behind-the-wheel</t>
+  </si>
+  <si>
+    <t>https://upgrade.qa4.jnj.psdops.com/our-company/johnsons-first-touch-infant-massage-event-a-guinness-world-records-victory</t>
+  </si>
+  <si>
+    <t>https://upgrade.qa4.jnj.psdops.com/caring-and-giving/johnsons-first-touch-infant-massage-event-a-guinness-world-records-victory</t>
+  </si>
+  <si>
+    <t>https://upgrade.qa4.jnj.psdops.com/caring-and-giving/seeking-todays-midwifery-pioneers-for-johnson-johnsons-genh-challenge</t>
+  </si>
+  <si>
+    <t>https://upgrade.qa4.jnj.psdops.com/our-company/seeking-todays-midwifery-pioneers-for-johnson-johnsons-genh-challenge</t>
+  </si>
+  <si>
+    <t>https://upgrade.qa4.jnj.psdops.com/caring-and-giving/icm-research-premieres-the-importance-of-sleep-on-social-emotional-development</t>
+  </si>
+  <si>
+    <t>https://upgrade.qa4.jnj.psdops.com/our-company/icm-research-premieres-the-importance-of-sleep-on-social-emotional-development</t>
+  </si>
+  <si>
+    <t>https://upgrade.qa4.jnj.psdops.com/icm-research-premieres-sleep-in-young-children-around-the-world</t>
+  </si>
+  <si>
+    <t>https://upgrade.qa4.jnj.psdops.com/our-company/icm-research-premieres-sleep-in-young-children-around-the-world</t>
+  </si>
+  <si>
+    <t>https://upgrade.qa4.jnj.psdops.com/caring-and-giving/midwives-lead-in-prevention-and-management-of-bleeding-after-birth</t>
+  </si>
+  <si>
+    <t>https://upgrade.qa4.jnj.psdops.com/our-company/midwives-lead-in-prevention-and-management-of-bleeding-after-birth</t>
+  </si>
+  <si>
+    <t>https://upgrade.qa4.jnj.psdops.com/caring-and-giving/midwives-video-5</t>
+  </si>
+  <si>
+    <t>https://upgrade.qa4.jnj.psdops.com/our-company/midwives-video-5</t>
+  </si>
+  <si>
+    <t>https://upgrade.qa4.jnj.psdops.com/caring-and-giving/midwives-lead-in-building-teams</t>
+  </si>
+  <si>
+    <t>https://upgrade.qa4.jnj.psdops.com/our-company/midwives-lead-in-building-teams</t>
+  </si>
+  <si>
+    <t>https://upgrade.qa4.jnj.psdops.com/caring-and-giving/midwives-lead-in-clinical-skills</t>
+  </si>
+  <si>
+    <t>https://upgrade.qa4.jnj.psdops.com/our-company/midwives-lead-in-clinical-skills</t>
+  </si>
+  <si>
+    <t>https://upgrade.qa4.jnj.psdops.com/caring-and-giving/midwives-video-2</t>
+  </si>
+  <si>
+    <t>https://upgrade.qa4.jnj.psdops.com/our-company/midwives-video-2</t>
+  </si>
+  <si>
+    <t>https://upgrade.qa4.jnj.psdops.com/caring-and-giving/midwives-video-1</t>
+  </si>
+  <si>
+    <t>https://upgrade.qa4.jnj.psdops.com/our-company/midwives-video-1</t>
+  </si>
+  <si>
+    <t>https://upgrade.qa4.jnj.psdops.com/new-ideas/building-the-confidence-of-a-new-generation-of-midwives-on-the-front-lines-of-care</t>
+  </si>
+  <si>
+    <t>https://upgrade.qa4.jnj.psdops.com/our-company/building-the-confidence-of-a-new-generation-of-midwives-on-the-front-lines-of-care</t>
   </si>
 </sst>
 </file>
@@ -7812,10 +7879,159 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B806BCDE-C70F-6D4A-BF69-E1B69B9EF7F2}">
+  <dimension ref="A1:A22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A1" s="9" t="s">
+        <v>2442</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A2" s="9" t="s">
+        <v>2443</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A3" s="9" t="s">
+        <v>2444</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A4" s="9" t="s">
+        <v>2445</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A5" s="9" t="s">
+        <v>2446</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A6" s="9" t="s">
+        <v>2447</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A7" s="9" t="s">
+        <v>2448</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A8" s="9" t="s">
+        <v>2449</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A9" s="9" t="s">
+        <v>2450</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A10" s="9" t="s">
+        <v>2451</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A11" s="9" t="s">
+        <v>2452</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A12" s="9" t="s">
+        <v>2453</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A13" s="9" t="s">
+        <v>2454</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A14" s="9" t="s">
+        <v>2455</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A15" s="9" t="s">
+        <v>2456</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A16" s="9" t="s">
+        <v>2457</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A17" s="9" t="s">
+        <v>2458</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A18" s="9" t="s">
+        <v>2459</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A19" s="9" t="s">
+        <v>2460</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A20" s="9" t="s">
+        <v>2461</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A21" s="9" t="s">
+        <v>2462</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A22" s="9" t="s">
+        <v>2463</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1" display="https://upgrade.qa4.jnj.psdops.com/cour-company/johnsons-first-touch-infant-massage-event-a-guinness-world-records-victory" xr:uid="{7950B623-1E77-0D4C-A004-7CCB7B5C4BCE}"/>
+    <hyperlink ref="A2" r:id="rId2" display="https://upgrade.qa4.jnj.psdops.com/ccaring-and-giving/johnsons-first-touch-infant-massage-event-a-guinness-world-records-victory" xr:uid="{08D726AB-6481-D44C-A807-DDF8DFB682F7}"/>
+    <hyperlink ref="A3" r:id="rId3" display="https://upgrade.qa4.jnj.psdops.com/ccaring-and-giving/seeking-todays-midwifery-pioneers-for-johnson-johnsons-genh-challenge" xr:uid="{4BB29CBF-AD0C-8B4B-BBBC-AD9D003311BD}"/>
+    <hyperlink ref="A4" r:id="rId4" xr:uid="{B613A96D-3233-B346-BEAD-16F77CBA0DBC}"/>
+    <hyperlink ref="A5" r:id="rId5" xr:uid="{EA07F56D-2518-4D4C-8962-403A8046FC48}"/>
+    <hyperlink ref="A6" r:id="rId6" xr:uid="{2EA9CC32-6148-2340-A8A2-0321626C8EEC}"/>
+    <hyperlink ref="A7" r:id="rId7" xr:uid="{664564DB-3D44-104C-BC51-1EB9420897A0}"/>
+    <hyperlink ref="A8" r:id="rId8" xr:uid="{8248E9F5-5511-1E46-B329-597480741C87}"/>
+    <hyperlink ref="A9" r:id="rId9" xr:uid="{02134FB0-DFF2-F34A-B844-7F53E0C3D700}"/>
+    <hyperlink ref="A10" r:id="rId10" xr:uid="{15725C8C-6E51-FD40-A6A6-5BE8A0F66CF7}"/>
+    <hyperlink ref="A11" r:id="rId11" xr:uid="{253B5697-B5C4-E64A-8DAE-64F75F7BAF22}"/>
+    <hyperlink ref="A12" r:id="rId12" xr:uid="{1D6C8FBB-4A55-DA4B-B835-567DC293283B}"/>
+    <hyperlink ref="A13" r:id="rId13" xr:uid="{2942D65C-F154-5844-8521-CC9713D004EA}"/>
+    <hyperlink ref="A14" r:id="rId14" xr:uid="{42A8D5A2-FBEE-B640-A25F-1DE49FE5CB30}"/>
+    <hyperlink ref="A15" r:id="rId15" xr:uid="{7E878D56-BEE6-A54A-96B5-A8563AE4A156}"/>
+    <hyperlink ref="A16" r:id="rId16" xr:uid="{286AF3FD-1B34-0341-854E-25BFDD20014F}"/>
+    <hyperlink ref="A17" r:id="rId17" xr:uid="{6876B8D8-4AA9-954F-82F5-3A96EB19DC94}"/>
+    <hyperlink ref="A18" r:id="rId18" xr:uid="{16A4CB0D-44ED-B748-BDE2-9EDB27BA9D01}"/>
+    <hyperlink ref="A19" r:id="rId19" xr:uid="{C283C5B5-43CB-2846-8141-9FE9926AA091}"/>
+    <hyperlink ref="A20" r:id="rId20" xr:uid="{B5E6B9D0-3798-F644-A092-CBC5DB3EDB4A}"/>
+    <hyperlink ref="A21" r:id="rId21" xr:uid="{539BBEAF-D26B-B24F-9230-FF7391ABBBBE}"/>
+    <hyperlink ref="A22" r:id="rId22" xr:uid="{C2CC9794-2F6B-1941-9446-588CE12C6EDA}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A62447A-6D9F-DD47-A3BC-B618ADF8CB98}">
   <dimension ref="A1:A300"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A252" workbookViewId="0">
+    <sheetView topLeftCell="A252" workbookViewId="0">
       <selection activeCell="A306" sqref="A306"/>
     </sheetView>
   </sheetViews>
@@ -9631,12 +9847,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C13CFE30-8DC9-8646-B751-1CC2599DD0A8}">
   <dimension ref="A1:A300"/>
   <sheetViews>
     <sheetView topLeftCell="A263" workbookViewId="0">
-      <selection activeCell="L306" sqref="L306"/>
+      <selection activeCell="B306" sqref="B306"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -11447,7 +11663,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA63C1F6-382A-F642-87F9-93CF1775AA78}">
   <dimension ref="A1:A300"/>
   <sheetViews>
@@ -13264,7 +13480,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0729FA2-658E-714E-BD63-184CECA54729}">
   <dimension ref="A1:A300"/>
   <sheetViews>
@@ -15081,7 +15297,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62F5E08C-0CC4-DF40-8568-D02DC4F72694}">
   <dimension ref="A1:A300"/>
   <sheetViews>
@@ -16898,7 +17114,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{020ABC0E-71DA-C24A-A601-CE49653F1796}">
   <dimension ref="A1:A270"/>
   <sheetViews>
@@ -18535,7 +18751,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>

</xml_diff>

<commit_message>
Added a new tab to experiment
</commit_message>
<xml_diff>
--- a/Redesign-Redirects.xlsx
+++ b/Redesign-Redirects.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sampanda/Samshub/test-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F947668C-3BFA-DE42-B5E7-71218F60143E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23802AC0-E142-D841-9089-8939C14F1C5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12340" yWindow="3220" windowWidth="32260" windowHeight="23640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Homepage-0" sheetId="8" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7104" uniqueCount="2466">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7092" uniqueCount="2444">
   <si>
     <t xml:space="preserve">Name of article </t>
   </si>
@@ -7464,72 +7464,6 @@
   </si>
   <si>
     <t>https://www.jnj.com/2011/10/drive-safely-work-week-and-btw-behind-the-wheel</t>
-  </si>
-  <si>
-    <t>https://upgrade.qa4.jnj.psdops.com/our-company/johnsons-first-touch-infant-massage-event-a-guinness-world-records-victory</t>
-  </si>
-  <si>
-    <t>https://upgrade.qa4.jnj.psdops.com/caring-and-giving/johnsons-first-touch-infant-massage-event-a-guinness-world-records-victory</t>
-  </si>
-  <si>
-    <t>https://upgrade.qa4.jnj.psdops.com/caring-and-giving/seeking-todays-midwifery-pioneers-for-johnson-johnsons-genh-challenge</t>
-  </si>
-  <si>
-    <t>https://upgrade.qa4.jnj.psdops.com/our-company/seeking-todays-midwifery-pioneers-for-johnson-johnsons-genh-challenge</t>
-  </si>
-  <si>
-    <t>https://upgrade.qa4.jnj.psdops.com/caring-and-giving/icm-research-premieres-the-importance-of-sleep-on-social-emotional-development</t>
-  </si>
-  <si>
-    <t>https://upgrade.qa4.jnj.psdops.com/our-company/icm-research-premieres-the-importance-of-sleep-on-social-emotional-development</t>
-  </si>
-  <si>
-    <t>https://upgrade.qa4.jnj.psdops.com/icm-research-premieres-sleep-in-young-children-around-the-world</t>
-  </si>
-  <si>
-    <t>https://upgrade.qa4.jnj.psdops.com/our-company/icm-research-premieres-sleep-in-young-children-around-the-world</t>
-  </si>
-  <si>
-    <t>https://upgrade.qa4.jnj.psdops.com/caring-and-giving/midwives-lead-in-prevention-and-management-of-bleeding-after-birth</t>
-  </si>
-  <si>
-    <t>https://upgrade.qa4.jnj.psdops.com/our-company/midwives-lead-in-prevention-and-management-of-bleeding-after-birth</t>
-  </si>
-  <si>
-    <t>https://upgrade.qa4.jnj.psdops.com/caring-and-giving/midwives-video-5</t>
-  </si>
-  <si>
-    <t>https://upgrade.qa4.jnj.psdops.com/our-company/midwives-video-5</t>
-  </si>
-  <si>
-    <t>https://upgrade.qa4.jnj.psdops.com/caring-and-giving/midwives-lead-in-building-teams</t>
-  </si>
-  <si>
-    <t>https://upgrade.qa4.jnj.psdops.com/our-company/midwives-lead-in-building-teams</t>
-  </si>
-  <si>
-    <t>https://upgrade.qa4.jnj.psdops.com/caring-and-giving/midwives-lead-in-clinical-skills</t>
-  </si>
-  <si>
-    <t>https://upgrade.qa4.jnj.psdops.com/our-company/midwives-lead-in-clinical-skills</t>
-  </si>
-  <si>
-    <t>https://upgrade.qa4.jnj.psdops.com/caring-and-giving/midwives-video-2</t>
-  </si>
-  <si>
-    <t>https://upgrade.qa4.jnj.psdops.com/our-company/midwives-video-2</t>
-  </si>
-  <si>
-    <t>https://upgrade.qa4.jnj.psdops.com/caring-and-giving/midwives-video-1</t>
-  </si>
-  <si>
-    <t>https://upgrade.qa4.jnj.psdops.com/our-company/midwives-video-1</t>
-  </si>
-  <si>
-    <t>https://upgrade.qa4.jnj.psdops.com/new-ideas/building-the-confidence-of-a-new-generation-of-midwives-on-the-front-lines-of-care</t>
-  </si>
-  <si>
-    <t>https://upgrade.qa4.jnj.psdops.com/our-company/building-the-confidence-of-a-new-generation-of-midwives-on-the-front-lines-of-care</t>
   </si>
   <si>
     <t>https://www.jnj.com/caring-and-giving/midwives-lead-in-building-teams</t>
@@ -7885,160 +7819,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B806BCDE-C70F-6D4A-BF69-E1B69B9EF7F2}">
-  <dimension ref="A1:A22"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A1" s="9" t="s">
-        <v>2442</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A2" s="9" t="s">
-        <v>2443</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A3" s="9" t="s">
-        <v>2444</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A4" s="9" t="s">
-        <v>2445</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A5" s="9" t="s">
-        <v>2446</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A6" s="9" t="s">
-        <v>2447</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A7" s="9" t="s">
-        <v>2448</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A8" s="9" t="s">
-        <v>2449</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A9" s="9" t="s">
-        <v>2450</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A10" s="9" t="s">
-        <v>2451</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A11" s="9" t="s">
-        <v>2452</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A12" s="9" t="s">
-        <v>2453</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A13" s="9" t="s">
-        <v>2454</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A14" s="9" t="s">
-        <v>2455</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A15" s="9" t="s">
-        <v>2456</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A16" s="9" t="s">
-        <v>2457</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A17" s="9" t="s">
-        <v>2458</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A18" s="9" t="s">
-        <v>2459</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A19" s="9" t="s">
-        <v>2460</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A20" s="9" t="s">
-        <v>2461</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A21" s="9" t="s">
-        <v>2462</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A22" s="9" t="s">
-        <v>2463</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" display="https://upgrade.qa4.jnj.psdops.com/cour-company/johnsons-first-touch-infant-massage-event-a-guinness-world-records-victory" xr:uid="{7950B623-1E77-0D4C-A004-7CCB7B5C4BCE}"/>
-    <hyperlink ref="A2" r:id="rId2" display="https://upgrade.qa4.jnj.psdops.com/ccaring-and-giving/johnsons-first-touch-infant-massage-event-a-guinness-world-records-victory" xr:uid="{08D726AB-6481-D44C-A807-DDF8DFB682F7}"/>
-    <hyperlink ref="A3" r:id="rId3" display="https://upgrade.qa4.jnj.psdops.com/ccaring-and-giving/seeking-todays-midwifery-pioneers-for-johnson-johnsons-genh-challenge" xr:uid="{4BB29CBF-AD0C-8B4B-BBBC-AD9D003311BD}"/>
-    <hyperlink ref="A4" r:id="rId4" xr:uid="{B613A96D-3233-B346-BEAD-16F77CBA0DBC}"/>
-    <hyperlink ref="A5" r:id="rId5" xr:uid="{EA07F56D-2518-4D4C-8962-403A8046FC48}"/>
-    <hyperlink ref="A6" r:id="rId6" xr:uid="{2EA9CC32-6148-2340-A8A2-0321626C8EEC}"/>
-    <hyperlink ref="A7" r:id="rId7" xr:uid="{664564DB-3D44-104C-BC51-1EB9420897A0}"/>
-    <hyperlink ref="A8" r:id="rId8" xr:uid="{8248E9F5-5511-1E46-B329-597480741C87}"/>
-    <hyperlink ref="A9" r:id="rId9" xr:uid="{02134FB0-DFF2-F34A-B844-7F53E0C3D700}"/>
-    <hyperlink ref="A10" r:id="rId10" xr:uid="{15725C8C-6E51-FD40-A6A6-5BE8A0F66CF7}"/>
-    <hyperlink ref="A11" r:id="rId11" xr:uid="{253B5697-B5C4-E64A-8DAE-64F75F7BAF22}"/>
-    <hyperlink ref="A12" r:id="rId12" xr:uid="{1D6C8FBB-4A55-DA4B-B835-567DC293283B}"/>
-    <hyperlink ref="A13" r:id="rId13" xr:uid="{2942D65C-F154-5844-8521-CC9713D004EA}"/>
-    <hyperlink ref="A14" r:id="rId14" xr:uid="{42A8D5A2-FBEE-B640-A25F-1DE49FE5CB30}"/>
-    <hyperlink ref="A15" r:id="rId15" xr:uid="{7E878D56-BEE6-A54A-96B5-A8563AE4A156}"/>
-    <hyperlink ref="A16" r:id="rId16" xr:uid="{286AF3FD-1B34-0341-854E-25BFDD20014F}"/>
-    <hyperlink ref="A17" r:id="rId17" xr:uid="{6876B8D8-4AA9-954F-82F5-3A96EB19DC94}"/>
-    <hyperlink ref="A18" r:id="rId18" xr:uid="{16A4CB0D-44ED-B748-BDE2-9EDB27BA9D01}"/>
-    <hyperlink ref="A19" r:id="rId19" xr:uid="{C283C5B5-43CB-2846-8141-9FE9926AA091}"/>
-    <hyperlink ref="A20" r:id="rId20" xr:uid="{B5E6B9D0-3798-F644-A092-CBC5DB3EDB4A}"/>
-    <hyperlink ref="A21" r:id="rId21" xr:uid="{539BBEAF-D26B-B24F-9230-FF7391ABBBBE}"/>
-    <hyperlink ref="A22" r:id="rId22" xr:uid="{C2CC9794-2F6B-1941-9446-588CE12C6EDA}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A62447A-6D9F-DD47-A3BC-B618ADF8CB98}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE2BFB8D-47AB-4E44-B28F-601BB38A8F99}">
   <dimension ref="A1:A300"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -8097,6 +7882,956 @@
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A11" s="9"/>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A12" s="9"/>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A13" s="9"/>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A14" s="9"/>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A15" s="9"/>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A16" s="9"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A17" s="9"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A18" s="9"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A19" s="9"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A20" s="9"/>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A21" s="9"/>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A22" s="9"/>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A23" s="9"/>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A24" s="9"/>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A25" s="9"/>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A26" s="9"/>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A27" s="9"/>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A28" s="9"/>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A29" s="9"/>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A30" s="9"/>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A31" s="9"/>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A32" s="9"/>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A33" s="9"/>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A34" s="9"/>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A35" s="9"/>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A36" s="9"/>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A37" s="9"/>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A38" s="9"/>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A39" s="9"/>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A40" s="9"/>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A41" s="9"/>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A42" s="9"/>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A43" s="9"/>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A44" s="9"/>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A45" s="9"/>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A46" s="9"/>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A47" s="9"/>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A48" s="9"/>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A49" s="9"/>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A50" s="9"/>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A51" s="9"/>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A52" s="9"/>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A53" s="9"/>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A54" s="9"/>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A55" s="9"/>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A56" s="9"/>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A57" s="9"/>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A58" s="9"/>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A59" s="9"/>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A60" s="9"/>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A61" s="9"/>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A62" s="9"/>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A63" s="9"/>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A64" s="9"/>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A65" s="9"/>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A66" s="9"/>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A67" s="9"/>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A68" s="9"/>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A69" s="9"/>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A70" s="9"/>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A71" s="9"/>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A72" s="9"/>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A73" s="9"/>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A74" s="9"/>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A75" s="9"/>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A76" s="9"/>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A77" s="9"/>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A78" s="9"/>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A79" s="9"/>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A80" s="9"/>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A81" s="9"/>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A82" s="9"/>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A83" s="9"/>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A84" s="9"/>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A85" s="9"/>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A86" s="9"/>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A87" s="9"/>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A88" s="9"/>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A89" s="9"/>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A90" s="9"/>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A91" s="9"/>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A92" s="9"/>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A93" s="9"/>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A94" s="9"/>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A95" s="9"/>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A96" s="9"/>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A97" s="9"/>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A98" s="9"/>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A99" s="9"/>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A100" s="9"/>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A101" s="9"/>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A102" s="9"/>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A103" s="9"/>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A104" s="9"/>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A105" s="9"/>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A106" s="9"/>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A107" s="9"/>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A108" s="9"/>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A109" s="9"/>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A110" s="9"/>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A111" s="9"/>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A112" s="9"/>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A113" s="9"/>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A114" s="9"/>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A115" s="9"/>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A116" s="9"/>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A117" s="9"/>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A118" s="9"/>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A119" s="9"/>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A120" s="9"/>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A121" s="9"/>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A122" s="9"/>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A123" s="9"/>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A124" s="9"/>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A125" s="9"/>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A126" s="9"/>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A127" s="9"/>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A128" s="9"/>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A129" s="9"/>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A130" s="9"/>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A131" s="9"/>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A132" s="9"/>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A133" s="9"/>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A134" s="9"/>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A135" s="9"/>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A136" s="9"/>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A137" s="9"/>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A138" s="9"/>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A139" s="9"/>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A140" s="9"/>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A141" s="9"/>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A142" s="9"/>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A143" s="9"/>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A144" s="9"/>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A145" s="9"/>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A146" s="9"/>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A147" s="9"/>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A148" s="9"/>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A149" s="9"/>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A150" s="9"/>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A151" s="9"/>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A152" s="9"/>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A153" s="9"/>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A154" s="9"/>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A155" s="9"/>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A156" s="9"/>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A157" s="9"/>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A158" s="9"/>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A159" s="9"/>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A160" s="9"/>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A161" s="9"/>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A162" s="9"/>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A163" s="9"/>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A164" s="9"/>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A165" s="9"/>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A166" s="9"/>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A167" s="9"/>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A168" s="9"/>
+    </row>
+    <row r="169" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A169" s="9"/>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A170" s="9"/>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A171" s="9"/>
+    </row>
+    <row r="172" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A172" s="9"/>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A173" s="9"/>
+    </row>
+    <row r="174" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A174" s="9"/>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A175" s="9"/>
+    </row>
+    <row r="176" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A176" s="9"/>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A177" s="9"/>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A178" s="9"/>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A179" s="9"/>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A180" s="9"/>
+    </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A181" s="9"/>
+    </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A182" s="9"/>
+    </row>
+    <row r="183" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A183" s="9"/>
+    </row>
+    <row r="184" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A184" s="9"/>
+    </row>
+    <row r="185" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A185" s="9"/>
+    </row>
+    <row r="186" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A186" s="9"/>
+    </row>
+    <row r="187" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A187" s="9"/>
+    </row>
+    <row r="188" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A188" s="9"/>
+    </row>
+    <row r="189" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A189" s="9"/>
+    </row>
+    <row r="190" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A190" s="9"/>
+    </row>
+    <row r="191" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A191" s="9"/>
+    </row>
+    <row r="192" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A192" s="9"/>
+    </row>
+    <row r="193" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A193" s="9"/>
+    </row>
+    <row r="194" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A194" s="9"/>
+    </row>
+    <row r="195" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A195" s="9"/>
+    </row>
+    <row r="196" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A196" s="9"/>
+    </row>
+    <row r="197" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A197" s="9"/>
+    </row>
+    <row r="198" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A198" s="9"/>
+    </row>
+    <row r="199" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A199" s="9"/>
+    </row>
+    <row r="200" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A200" s="9"/>
+    </row>
+    <row r="201" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A201" s="9"/>
+    </row>
+    <row r="202" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A202" s="9"/>
+    </row>
+    <row r="203" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A203" s="9"/>
+    </row>
+    <row r="204" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A204" s="9"/>
+    </row>
+    <row r="205" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A205" s="9"/>
+    </row>
+    <row r="206" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A206" s="9"/>
+    </row>
+    <row r="207" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A207" s="9"/>
+    </row>
+    <row r="208" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A208" s="9"/>
+    </row>
+    <row r="209" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A209" s="9"/>
+    </row>
+    <row r="210" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A210" s="9"/>
+    </row>
+    <row r="211" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A211" s="9"/>
+    </row>
+    <row r="212" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A212" s="9"/>
+    </row>
+    <row r="213" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A213" s="9"/>
+    </row>
+    <row r="214" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A214" s="9"/>
+    </row>
+    <row r="215" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A215" s="9"/>
+    </row>
+    <row r="216" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A216" s="9"/>
+    </row>
+    <row r="217" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A217" s="9"/>
+    </row>
+    <row r="218" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A218" s="9"/>
+    </row>
+    <row r="219" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A219" s="9"/>
+    </row>
+    <row r="220" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A220" s="9"/>
+    </row>
+    <row r="221" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A221" s="9"/>
+    </row>
+    <row r="222" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A222" s="9"/>
+    </row>
+    <row r="223" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A223" s="9"/>
+    </row>
+    <row r="224" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A224" s="9"/>
+    </row>
+    <row r="225" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A225" s="9"/>
+    </row>
+    <row r="226" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A226" s="9"/>
+    </row>
+    <row r="227" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A227" s="9"/>
+    </row>
+    <row r="228" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A228" s="9"/>
+    </row>
+    <row r="229" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A229" s="9"/>
+    </row>
+    <row r="230" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A230" s="9"/>
+    </row>
+    <row r="231" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A231" s="9"/>
+    </row>
+    <row r="232" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A232" s="9"/>
+    </row>
+    <row r="233" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A233" s="9"/>
+    </row>
+    <row r="234" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A234" s="9"/>
+    </row>
+    <row r="235" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A235" s="9"/>
+    </row>
+    <row r="236" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A236" s="9"/>
+    </row>
+    <row r="237" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A237" s="9"/>
+    </row>
+    <row r="238" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A238" s="9"/>
+    </row>
+    <row r="239" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A239" s="9"/>
+    </row>
+    <row r="240" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A240" s="9"/>
+    </row>
+    <row r="241" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A241" s="9"/>
+    </row>
+    <row r="242" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A242" s="9"/>
+    </row>
+    <row r="243" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A243" s="9"/>
+    </row>
+    <row r="244" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A244" s="9"/>
+    </row>
+    <row r="245" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A245" s="9"/>
+    </row>
+    <row r="246" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A246" s="9"/>
+    </row>
+    <row r="247" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A247" s="9"/>
+    </row>
+    <row r="248" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A248" s="9"/>
+    </row>
+    <row r="249" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A249" s="9"/>
+    </row>
+    <row r="250" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A250" s="9"/>
+    </row>
+    <row r="251" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A251" s="9"/>
+    </row>
+    <row r="252" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A252" s="9"/>
+    </row>
+    <row r="253" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A253" s="9"/>
+    </row>
+    <row r="254" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A254" s="9"/>
+    </row>
+    <row r="255" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A255" s="9"/>
+    </row>
+    <row r="256" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A256" s="9"/>
+    </row>
+    <row r="257" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A257" s="9"/>
+    </row>
+    <row r="258" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A258" s="9"/>
+    </row>
+    <row r="259" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A259" s="9"/>
+    </row>
+    <row r="260" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A260" s="9"/>
+    </row>
+    <row r="261" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A261" s="9"/>
+    </row>
+    <row r="262" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A262" s="9"/>
+    </row>
+    <row r="263" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A263" s="9"/>
+    </row>
+    <row r="264" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A264" s="9"/>
+    </row>
+    <row r="265" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A265" s="9"/>
+    </row>
+    <row r="266" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A266" s="9"/>
+    </row>
+    <row r="267" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A267" s="9"/>
+    </row>
+    <row r="268" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A268" s="9"/>
+    </row>
+    <row r="269" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A269" s="9"/>
+    </row>
+    <row r="270" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A270" s="9"/>
+    </row>
+    <row r="271" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A271" s="9"/>
+    </row>
+    <row r="272" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A272" s="9"/>
+    </row>
+    <row r="273" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A273" s="9"/>
+    </row>
+    <row r="274" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A274" s="9"/>
+    </row>
+    <row r="275" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A275" s="9"/>
+    </row>
+    <row r="276" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A276" s="9"/>
+    </row>
+    <row r="277" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A277" s="9"/>
+    </row>
+    <row r="278" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A278" s="9"/>
+    </row>
+    <row r="279" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A279" s="9"/>
+    </row>
+    <row r="280" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A280" s="9"/>
+    </row>
+    <row r="281" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A281" s="9"/>
+    </row>
+    <row r="282" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A282" s="9"/>
+    </row>
+    <row r="283" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A283" s="9"/>
+    </row>
+    <row r="284" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A284" s="9"/>
+    </row>
+    <row r="285" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A285" s="9"/>
+    </row>
+    <row r="286" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A286" s="9"/>
+    </row>
+    <row r="287" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A287" s="9"/>
+    </row>
+    <row r="288" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A288" s="9"/>
+    </row>
+    <row r="289" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A289" s="9"/>
+    </row>
+    <row r="290" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A290" s="9"/>
+    </row>
+    <row r="291" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A291" s="9"/>
+    </row>
+    <row r="292" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A292" s="9"/>
+    </row>
+    <row r="293" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A293" s="9"/>
+    </row>
+    <row r="294" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A294" s="9"/>
+    </row>
+    <row r="295" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A295" s="9"/>
+    </row>
+    <row r="296" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A296" s="9"/>
+    </row>
+    <row r="297" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A297" s="9"/>
+    </row>
+    <row r="298" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A298" s="9"/>
+    </row>
+    <row r="299" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A299" s="9"/>
+    </row>
+    <row r="300" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A300" s="4"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1" xr:uid="{CD93644A-E5A6-024D-8891-D4268023C180}"/>
+    <hyperlink ref="A2" r:id="rId2" xr:uid="{7B46CF00-7058-764C-ADA5-BC3BF1729BB8}"/>
+    <hyperlink ref="A3" r:id="rId3" xr:uid="{F09BCE01-9BF9-AB49-9B6E-BAC69F63F074}"/>
+    <hyperlink ref="A4" r:id="rId4" xr:uid="{2EEA14F5-8F8E-3748-800A-785E866C392E}"/>
+    <hyperlink ref="A5" r:id="rId5" xr:uid="{ED6744D1-2E31-4349-9B67-B509C8B45DC3}"/>
+    <hyperlink ref="A6" r:id="rId6" xr:uid="{B0164AD7-23A2-FC4B-AD5A-15C1C2A707D4}"/>
+    <hyperlink ref="A7" r:id="rId7" xr:uid="{4642DB04-0726-DB4D-A76A-39874ADEF17A}"/>
+    <hyperlink ref="A8" r:id="rId8" xr:uid="{0AA588E9-C54B-0143-89C7-EFDA53353888}"/>
+    <hyperlink ref="A9" r:id="rId9" xr:uid="{11D43C14-6D66-8E4E-B20C-576834224A80}"/>
+    <hyperlink ref="A10" r:id="rId10" xr:uid="{5FDCC4A1-2A77-1548-A805-D4B7D3865348}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A62447A-6D9F-DD47-A3BC-B618ADF8CB98}">
+  <dimension ref="A1:A300"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A301" sqref="A301"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="105.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A1" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A2" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A3" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A4" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A5" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A6" s="9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A7" s="9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A8" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A9" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A10" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A11" s="9" t="s">
         <v>21</v>
       </c>
@@ -8108,7 +8843,7 @@
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A13" s="9" t="s">
-        <v>2464</v>
+        <v>2442</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.15">
@@ -8963,7 +9698,7 @@
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A184" s="9" t="s">
-        <v>2465</v>
+        <v>2443</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.15">
@@ -9854,8 +10589,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C13CFE30-8DC9-8646-B751-1CC2599DD0A8}">
   <dimension ref="A1:A300"/>
   <sheetViews>
-    <sheetView topLeftCell="A263" workbookViewId="0">
-      <selection activeCell="B306" sqref="B306"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N26" sqref="N26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -17122,7 +17857,7 @@
   <dimension ref="A1:A270"/>
   <sheetViews>
     <sheetView topLeftCell="A217" workbookViewId="0">
-      <selection activeCell="K232" sqref="K232"/>
+      <selection activeCell="X217" sqref="X1:X1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
Remove dupilcates from Homepage-6 tab
</commit_message>
<xml_diff>
--- a/Redesign-Redirects.xlsx
+++ b/Redesign-Redirects.xlsx
@@ -8,26 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sampanda/Samshub/test-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23802AC0-E142-D841-9089-8939C14F1C5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73ED6D55-A488-7348-B9D3-12B3CFD74A7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="31680" windowHeight="21280" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Homepage-0" sheetId="8" r:id="rId1"/>
-    <sheet name="Homepage-1" sheetId="2" r:id="rId2"/>
-    <sheet name="Homepage-2" sheetId="3" r:id="rId3"/>
-    <sheet name="Homepage-3" sheetId="4" r:id="rId4"/>
-    <sheet name="Homepage-4" sheetId="5" r:id="rId5"/>
-    <sheet name="Homepage-5" sheetId="6" r:id="rId6"/>
-    <sheet name="Homepage-6" sheetId="7" r:id="rId7"/>
-    <sheet name="JNJ OUR COMPANYPRODUCT URL CLEA" sheetId="1" r:id="rId8"/>
+    <sheet name="Homepage-1" sheetId="2" r:id="rId1"/>
+    <sheet name="Homepage-2" sheetId="3" r:id="rId2"/>
+    <sheet name="Homepage-3" sheetId="4" r:id="rId3"/>
+    <sheet name="Homepage-4" sheetId="5" r:id="rId4"/>
+    <sheet name="Homepage-5" sheetId="6" r:id="rId5"/>
+    <sheet name="Homepage-6" sheetId="7" r:id="rId6"/>
+    <sheet name="JNJ OUR COMPANYPRODUCT URL CLEA" sheetId="1" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7092" uniqueCount="2444">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7079" uniqueCount="2444">
   <si>
     <t xml:space="preserve">Name of article </t>
   </si>
@@ -7819,960 +7818,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE2BFB8D-47AB-4E44-B28F-601BB38A8F99}">
-  <dimension ref="A1:A300"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="1" max="1" width="105.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A1" s="9" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A2" s="9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A3" s="9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A4" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A5" s="9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A6" s="9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A7" s="9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A8" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A9" s="9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A10" s="9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A11" s="9"/>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A12" s="9"/>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A13" s="9"/>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A14" s="9"/>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A15" s="9"/>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A16" s="9"/>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A17" s="9"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A18" s="9"/>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A19" s="9"/>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A20" s="9"/>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A21" s="9"/>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A22" s="9"/>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A23" s="9"/>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A24" s="9"/>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A25" s="9"/>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A26" s="9"/>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A27" s="9"/>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A28" s="9"/>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A29" s="9"/>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A30" s="9"/>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A31" s="9"/>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A32" s="9"/>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A33" s="9"/>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A34" s="9"/>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A35" s="9"/>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A36" s="9"/>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A37" s="9"/>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A38" s="9"/>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A39" s="9"/>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A40" s="9"/>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A41" s="9"/>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A42" s="9"/>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A43" s="9"/>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A44" s="9"/>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A45" s="9"/>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A46" s="9"/>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A47" s="9"/>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A48" s="9"/>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A49" s="9"/>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A50" s="9"/>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A51" s="9"/>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A52" s="9"/>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A53" s="9"/>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A54" s="9"/>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A55" s="9"/>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A56" s="9"/>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A57" s="9"/>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A58" s="9"/>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A59" s="9"/>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A60" s="9"/>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A61" s="9"/>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A62" s="9"/>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A63" s="9"/>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A64" s="9"/>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A65" s="9"/>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A66" s="9"/>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A67" s="9"/>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A68" s="9"/>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A69" s="9"/>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A70" s="9"/>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A71" s="9"/>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A72" s="9"/>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A73" s="9"/>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A74" s="9"/>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A75" s="9"/>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A76" s="9"/>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A77" s="9"/>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A78" s="9"/>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A79" s="9"/>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A80" s="9"/>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A81" s="9"/>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A82" s="9"/>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A83" s="9"/>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A84" s="9"/>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A85" s="9"/>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A86" s="9"/>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A87" s="9"/>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A88" s="9"/>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A89" s="9"/>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A90" s="9"/>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A91" s="9"/>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A92" s="9"/>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A93" s="9"/>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A94" s="9"/>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A95" s="9"/>
-    </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A96" s="9"/>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A97" s="9"/>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A98" s="9"/>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A99" s="9"/>
-    </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A100" s="9"/>
-    </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A101" s="9"/>
-    </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A102" s="9"/>
-    </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A103" s="9"/>
-    </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A104" s="9"/>
-    </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A105" s="9"/>
-    </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A106" s="9"/>
-    </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A107" s="9"/>
-    </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A108" s="9"/>
-    </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A109" s="9"/>
-    </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A110" s="9"/>
-    </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A111" s="9"/>
-    </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A112" s="9"/>
-    </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A113" s="9"/>
-    </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A114" s="9"/>
-    </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A115" s="9"/>
-    </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A116" s="9"/>
-    </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A117" s="9"/>
-    </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A118" s="9"/>
-    </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A119" s="9"/>
-    </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A120" s="9"/>
-    </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A121" s="9"/>
-    </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A122" s="9"/>
-    </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A123" s="9"/>
-    </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A124" s="9"/>
-    </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A125" s="9"/>
-    </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A126" s="9"/>
-    </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A127" s="9"/>
-    </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A128" s="9"/>
-    </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A129" s="9"/>
-    </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A130" s="9"/>
-    </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A131" s="9"/>
-    </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A132" s="9"/>
-    </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A133" s="9"/>
-    </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A134" s="9"/>
-    </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A135" s="9"/>
-    </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A136" s="9"/>
-    </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A137" s="9"/>
-    </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A138" s="9"/>
-    </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A139" s="9"/>
-    </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A140" s="9"/>
-    </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A141" s="9"/>
-    </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A142" s="9"/>
-    </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A143" s="9"/>
-    </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A144" s="9"/>
-    </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A145" s="9"/>
-    </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A146" s="9"/>
-    </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A147" s="9"/>
-    </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A148" s="9"/>
-    </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A149" s="9"/>
-    </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A150" s="9"/>
-    </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A151" s="9"/>
-    </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A152" s="9"/>
-    </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A153" s="9"/>
-    </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A154" s="9"/>
-    </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A155" s="9"/>
-    </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A156" s="9"/>
-    </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A157" s="9"/>
-    </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A158" s="9"/>
-    </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A159" s="9"/>
-    </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A160" s="9"/>
-    </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A161" s="9"/>
-    </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A162" s="9"/>
-    </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A163" s="9"/>
-    </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A164" s="9"/>
-    </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A165" s="9"/>
-    </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A166" s="9"/>
-    </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A167" s="9"/>
-    </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A168" s="9"/>
-    </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A169" s="9"/>
-    </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A170" s="9"/>
-    </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A171" s="9"/>
-    </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A172" s="9"/>
-    </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A173" s="9"/>
-    </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A174" s="9"/>
-    </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A175" s="9"/>
-    </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A176" s="9"/>
-    </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A177" s="9"/>
-    </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A178" s="9"/>
-    </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A179" s="9"/>
-    </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A180" s="9"/>
-    </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A181" s="9"/>
-    </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A182" s="9"/>
-    </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A183" s="9"/>
-    </row>
-    <row r="184" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A184" s="9"/>
-    </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A185" s="9"/>
-    </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A186" s="9"/>
-    </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A187" s="9"/>
-    </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A188" s="9"/>
-    </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A189" s="9"/>
-    </row>
-    <row r="190" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A190" s="9"/>
-    </row>
-    <row r="191" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A191" s="9"/>
-    </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A192" s="9"/>
-    </row>
-    <row r="193" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A193" s="9"/>
-    </row>
-    <row r="194" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A194" s="9"/>
-    </row>
-    <row r="195" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A195" s="9"/>
-    </row>
-    <row r="196" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A196" s="9"/>
-    </row>
-    <row r="197" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A197" s="9"/>
-    </row>
-    <row r="198" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A198" s="9"/>
-    </row>
-    <row r="199" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A199" s="9"/>
-    </row>
-    <row r="200" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A200" s="9"/>
-    </row>
-    <row r="201" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A201" s="9"/>
-    </row>
-    <row r="202" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A202" s="9"/>
-    </row>
-    <row r="203" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A203" s="9"/>
-    </row>
-    <row r="204" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A204" s="9"/>
-    </row>
-    <row r="205" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A205" s="9"/>
-    </row>
-    <row r="206" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A206" s="9"/>
-    </row>
-    <row r="207" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A207" s="9"/>
-    </row>
-    <row r="208" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A208" s="9"/>
-    </row>
-    <row r="209" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A209" s="9"/>
-    </row>
-    <row r="210" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A210" s="9"/>
-    </row>
-    <row r="211" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A211" s="9"/>
-    </row>
-    <row r="212" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A212" s="9"/>
-    </row>
-    <row r="213" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A213" s="9"/>
-    </row>
-    <row r="214" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A214" s="9"/>
-    </row>
-    <row r="215" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A215" s="9"/>
-    </row>
-    <row r="216" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A216" s="9"/>
-    </row>
-    <row r="217" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A217" s="9"/>
-    </row>
-    <row r="218" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A218" s="9"/>
-    </row>
-    <row r="219" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A219" s="9"/>
-    </row>
-    <row r="220" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A220" s="9"/>
-    </row>
-    <row r="221" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A221" s="9"/>
-    </row>
-    <row r="222" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A222" s="9"/>
-    </row>
-    <row r="223" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A223" s="9"/>
-    </row>
-    <row r="224" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A224" s="9"/>
-    </row>
-    <row r="225" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A225" s="9"/>
-    </row>
-    <row r="226" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A226" s="9"/>
-    </row>
-    <row r="227" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A227" s="9"/>
-    </row>
-    <row r="228" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A228" s="9"/>
-    </row>
-    <row r="229" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A229" s="9"/>
-    </row>
-    <row r="230" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A230" s="9"/>
-    </row>
-    <row r="231" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A231" s="9"/>
-    </row>
-    <row r="232" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A232" s="9"/>
-    </row>
-    <row r="233" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A233" s="9"/>
-    </row>
-    <row r="234" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A234" s="9"/>
-    </row>
-    <row r="235" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A235" s="9"/>
-    </row>
-    <row r="236" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A236" s="9"/>
-    </row>
-    <row r="237" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A237" s="9"/>
-    </row>
-    <row r="238" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A238" s="9"/>
-    </row>
-    <row r="239" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A239" s="9"/>
-    </row>
-    <row r="240" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A240" s="9"/>
-    </row>
-    <row r="241" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A241" s="9"/>
-    </row>
-    <row r="242" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A242" s="9"/>
-    </row>
-    <row r="243" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A243" s="9"/>
-    </row>
-    <row r="244" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A244" s="9"/>
-    </row>
-    <row r="245" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A245" s="9"/>
-    </row>
-    <row r="246" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A246" s="9"/>
-    </row>
-    <row r="247" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A247" s="9"/>
-    </row>
-    <row r="248" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A248" s="9"/>
-    </row>
-    <row r="249" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A249" s="9"/>
-    </row>
-    <row r="250" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A250" s="9"/>
-    </row>
-    <row r="251" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A251" s="9"/>
-    </row>
-    <row r="252" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A252" s="9"/>
-    </row>
-    <row r="253" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A253" s="9"/>
-    </row>
-    <row r="254" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A254" s="9"/>
-    </row>
-    <row r="255" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A255" s="9"/>
-    </row>
-    <row r="256" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A256" s="9"/>
-    </row>
-    <row r="257" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A257" s="9"/>
-    </row>
-    <row r="258" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A258" s="9"/>
-    </row>
-    <row r="259" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A259" s="9"/>
-    </row>
-    <row r="260" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A260" s="9"/>
-    </row>
-    <row r="261" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A261" s="9"/>
-    </row>
-    <row r="262" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A262" s="9"/>
-    </row>
-    <row r="263" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A263" s="9"/>
-    </row>
-    <row r="264" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A264" s="9"/>
-    </row>
-    <row r="265" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A265" s="9"/>
-    </row>
-    <row r="266" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A266" s="9"/>
-    </row>
-    <row r="267" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A267" s="9"/>
-    </row>
-    <row r="268" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A268" s="9"/>
-    </row>
-    <row r="269" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A269" s="9"/>
-    </row>
-    <row r="270" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A270" s="9"/>
-    </row>
-    <row r="271" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A271" s="9"/>
-    </row>
-    <row r="272" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A272" s="9"/>
-    </row>
-    <row r="273" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A273" s="9"/>
-    </row>
-    <row r="274" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A274" s="9"/>
-    </row>
-    <row r="275" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A275" s="9"/>
-    </row>
-    <row r="276" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A276" s="9"/>
-    </row>
-    <row r="277" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A277" s="9"/>
-    </row>
-    <row r="278" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A278" s="9"/>
-    </row>
-    <row r="279" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A279" s="9"/>
-    </row>
-    <row r="280" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A280" s="9"/>
-    </row>
-    <row r="281" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A281" s="9"/>
-    </row>
-    <row r="282" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A282" s="9"/>
-    </row>
-    <row r="283" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A283" s="9"/>
-    </row>
-    <row r="284" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A284" s="9"/>
-    </row>
-    <row r="285" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A285" s="9"/>
-    </row>
-    <row r="286" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A286" s="9"/>
-    </row>
-    <row r="287" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A287" s="9"/>
-    </row>
-    <row r="288" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A288" s="9"/>
-    </row>
-    <row r="289" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A289" s="9"/>
-    </row>
-    <row r="290" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A290" s="9"/>
-    </row>
-    <row r="291" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A291" s="9"/>
-    </row>
-    <row r="292" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A292" s="9"/>
-    </row>
-    <row r="293" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A293" s="9"/>
-    </row>
-    <row r="294" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A294" s="9"/>
-    </row>
-    <row r="295" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A295" s="9"/>
-    </row>
-    <row r="296" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A296" s="9"/>
-    </row>
-    <row r="297" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A297" s="9"/>
-    </row>
-    <row r="298" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A298" s="9"/>
-    </row>
-    <row r="299" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A299" s="9"/>
-    </row>
-    <row r="300" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A300" s="4"/>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" xr:uid="{CD93644A-E5A6-024D-8891-D4268023C180}"/>
-    <hyperlink ref="A2" r:id="rId2" xr:uid="{7B46CF00-7058-764C-ADA5-BC3BF1729BB8}"/>
-    <hyperlink ref="A3" r:id="rId3" xr:uid="{F09BCE01-9BF9-AB49-9B6E-BAC69F63F074}"/>
-    <hyperlink ref="A4" r:id="rId4" xr:uid="{2EEA14F5-8F8E-3748-800A-785E866C392E}"/>
-    <hyperlink ref="A5" r:id="rId5" xr:uid="{ED6744D1-2E31-4349-9B67-B509C8B45DC3}"/>
-    <hyperlink ref="A6" r:id="rId6" xr:uid="{B0164AD7-23A2-FC4B-AD5A-15C1C2A707D4}"/>
-    <hyperlink ref="A7" r:id="rId7" xr:uid="{4642DB04-0726-DB4D-A76A-39874ADEF17A}"/>
-    <hyperlink ref="A8" r:id="rId8" xr:uid="{0AA588E9-C54B-0143-89C7-EFDA53353888}"/>
-    <hyperlink ref="A9" r:id="rId9" xr:uid="{11D43C14-6D66-8E4E-B20C-576834224A80}"/>
-    <hyperlink ref="A10" r:id="rId10" xr:uid="{5FDCC4A1-2A77-1548-A805-D4B7D3865348}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A62447A-6D9F-DD47-A3BC-B618ADF8CB98}">
   <dimension ref="A1:A300"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A285" workbookViewId="0">
       <selection activeCell="A301" sqref="A301"/>
     </sheetView>
   </sheetViews>
@@ -10585,11 +9634,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C13CFE30-8DC9-8646-B751-1CC2599DD0A8}">
   <dimension ref="A1:A300"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A259" workbookViewId="0">
       <selection activeCell="N26" sqref="N26"/>
     </sheetView>
   </sheetViews>
@@ -12401,11 +11450,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA63C1F6-382A-F642-87F9-93CF1775AA78}">
   <dimension ref="A1:A300"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A207" workbookViewId="0">
       <selection activeCell="K60" sqref="K60"/>
     </sheetView>
   </sheetViews>
@@ -14218,7 +13267,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0729FA2-658E-714E-BD63-184CECA54729}">
   <dimension ref="A1:A300"/>
   <sheetViews>
@@ -16035,7 +15084,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62F5E08C-0CC4-DF40-8568-D02DC4F72694}">
   <dimension ref="A1:A300"/>
   <sheetViews>
@@ -17852,15 +16901,18 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{020ABC0E-71DA-C24A-A601-CE49653F1796}">
-  <dimension ref="A1:A270"/>
+  <dimension ref="A1:A267"/>
   <sheetViews>
-    <sheetView topLeftCell="A217" workbookViewId="0">
-      <selection activeCell="X217" sqref="X1:X1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="A125" sqref="A125:XFD125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="126.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
@@ -18484,731 +17536,716 @@
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A125" s="4" t="s">
-        <v>1053</v>
+        <v>2249</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A126" s="4" t="s">
-        <v>1054</v>
+        <v>2250</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A127" s="4" t="s">
-        <v>1055</v>
+        <v>2252</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A128" s="4" t="s">
-        <v>2249</v>
+        <v>2253</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A129" s="4" t="s">
-        <v>2250</v>
+        <v>2254</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A130" s="4" t="s">
-        <v>2252</v>
+        <v>2256</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A131" s="4" t="s">
-        <v>2253</v>
+        <v>2258</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A132" s="4" t="s">
-        <v>2254</v>
+        <v>2259</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A133" s="4" t="s">
-        <v>2256</v>
+        <v>2260</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A134" s="4" t="s">
-        <v>2258</v>
+        <v>2262</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A135" s="4" t="s">
-        <v>2259</v>
+        <v>2263</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A136" s="4" t="s">
-        <v>2260</v>
+        <v>2264</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A137" s="4" t="s">
-        <v>2262</v>
+        <v>2266</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A138" s="4" t="s">
-        <v>2263</v>
+        <v>2267</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A139" s="4" t="s">
-        <v>2264</v>
+        <v>2268</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A140" s="4" t="s">
-        <v>2266</v>
+        <v>2270</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A141" s="4" t="s">
-        <v>2267</v>
+        <v>2271</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A142" s="4" t="s">
-        <v>2268</v>
+        <v>2272</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A143" s="4" t="s">
-        <v>2270</v>
+        <v>2274</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A144" s="4" t="s">
-        <v>2271</v>
+        <v>2275</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A145" s="4" t="s">
-        <v>2272</v>
+        <v>2276</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A146" s="4" t="s">
-        <v>2274</v>
+        <v>2278</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A147" s="4" t="s">
-        <v>2275</v>
+        <v>2278</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A148" s="4" t="s">
-        <v>2276</v>
+        <v>2280</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A149" s="4" t="s">
-        <v>2278</v>
+        <v>2281</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A150" s="4" t="s">
-        <v>2278</v>
+        <v>2282</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A151" s="4" t="s">
-        <v>2280</v>
+        <v>2284</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A152" s="4" t="s">
-        <v>2281</v>
+        <v>2285</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A153" s="4" t="s">
-        <v>2282</v>
+        <v>2286</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A154" s="4" t="s">
-        <v>2284</v>
+        <v>2288</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A155" s="4" t="s">
-        <v>2285</v>
+        <v>2289</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A156" s="4" t="s">
-        <v>2286</v>
+        <v>2290</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A157" s="4" t="s">
-        <v>2288</v>
+        <v>2292</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A158" s="4" t="s">
-        <v>2289</v>
+        <v>2293</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A159" s="4" t="s">
-        <v>2290</v>
+        <v>2294</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A160" s="4" t="s">
-        <v>2292</v>
+        <v>2296</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A161" s="4" t="s">
-        <v>2293</v>
+        <v>2297</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A162" s="4" t="s">
-        <v>2294</v>
+        <v>2298</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A163" s="4" t="s">
-        <v>2296</v>
+        <v>2300</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A164" s="4" t="s">
-        <v>2297</v>
+        <v>2301</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A165" s="4" t="s">
-        <v>2298</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A166" s="4" t="s">
-        <v>2300</v>
+        <v>2304</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A167" s="4" t="s">
-        <v>2301</v>
+        <v>2305</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A168" s="4" t="s">
-        <v>2302</v>
+        <v>2306</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A169" s="4" t="s">
-        <v>2304</v>
+        <v>2308</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A170" s="4" t="s">
-        <v>2305</v>
+        <v>2309</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A171" s="4" t="s">
-        <v>2306</v>
+        <v>2310</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A172" s="4" t="s">
-        <v>2308</v>
+        <v>2312</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A173" s="4" t="s">
-        <v>2309</v>
+        <v>2313</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A174" s="4" t="s">
-        <v>2310</v>
+        <v>2314</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A175" s="4" t="s">
-        <v>2312</v>
+        <v>2316</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A176" s="4" t="s">
-        <v>2313</v>
+        <v>2317</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A177" s="4" t="s">
-        <v>2314</v>
+        <v>2319</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A178" s="4" t="s">
-        <v>2316</v>
+        <v>2320</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A179" s="4" t="s">
-        <v>2317</v>
+        <v>2321</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A180" s="4" t="s">
-        <v>2319</v>
+        <v>2323</v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A181" s="4" t="s">
-        <v>2320</v>
+        <v>2324</v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A182" s="4" t="s">
-        <v>2321</v>
+        <v>2325</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A183" s="4" t="s">
-        <v>2323</v>
+        <v>2327</v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A184" s="4" t="s">
-        <v>2324</v>
+        <v>2328</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A185" s="4" t="s">
-        <v>2325</v>
+        <v>2329</v>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A186" s="4" t="s">
-        <v>2327</v>
+        <v>2331</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A187" s="4" t="s">
-        <v>2328</v>
+        <v>2332</v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A188" s="4" t="s">
-        <v>2329</v>
+        <v>2333</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A189" s="4" t="s">
-        <v>2331</v>
+        <v>2335</v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A190" s="4" t="s">
-        <v>2332</v>
+        <v>2336</v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A191" s="4" t="s">
-        <v>2333</v>
+        <v>2337</v>
       </c>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A192" s="4" t="s">
-        <v>2335</v>
+        <v>2339</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A193" s="4" t="s">
-        <v>2336</v>
+        <v>2340</v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A194" s="4" t="s">
-        <v>2337</v>
+        <v>2341</v>
       </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A195" s="4" t="s">
-        <v>2339</v>
+        <v>2343</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A196" s="4" t="s">
-        <v>2340</v>
+        <v>2344</v>
       </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A197" s="4" t="s">
-        <v>2341</v>
+        <v>2345</v>
       </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A198" s="4" t="s">
-        <v>2343</v>
+        <v>2347</v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A199" s="4" t="s">
-        <v>2344</v>
+        <v>2348</v>
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A200" s="4" t="s">
-        <v>2345</v>
+        <v>2349</v>
       </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A201" s="4" t="s">
-        <v>2347</v>
+        <v>2351</v>
       </c>
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A202" s="4" t="s">
-        <v>2348</v>
+        <v>2352</v>
       </c>
     </row>
     <row r="203" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A203" s="4" t="s">
-        <v>2349</v>
+        <v>2353</v>
       </c>
     </row>
     <row r="204" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A204" s="4" t="s">
-        <v>2351</v>
+        <v>2355</v>
       </c>
     </row>
     <row r="205" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A205" s="4" t="s">
-        <v>2352</v>
+        <v>2356</v>
       </c>
     </row>
     <row r="206" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A206" s="4" t="s">
-        <v>2353</v>
+        <v>2357</v>
       </c>
     </row>
     <row r="207" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A207" s="4" t="s">
-        <v>2355</v>
+        <v>2359</v>
       </c>
     </row>
     <row r="208" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A208" s="4" t="s">
-        <v>2356</v>
+        <v>2360</v>
       </c>
     </row>
     <row r="209" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A209" s="4" t="s">
-        <v>2357</v>
+        <v>2361</v>
       </c>
     </row>
     <row r="210" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A210" s="4" t="s">
-        <v>2359</v>
+        <v>2363</v>
       </c>
     </row>
     <row r="211" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A211" s="4" t="s">
-        <v>2360</v>
+        <v>2364</v>
       </c>
     </row>
     <row r="212" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A212" s="4" t="s">
-        <v>2361</v>
+        <v>2365</v>
       </c>
     </row>
     <row r="213" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A213" s="4" t="s">
-        <v>2363</v>
+        <v>2367</v>
       </c>
     </row>
     <row r="214" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A214" s="4" t="s">
-        <v>2364</v>
+        <v>2368</v>
       </c>
     </row>
     <row r="215" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A215" s="4" t="s">
-        <v>2365</v>
+        <v>2369</v>
       </c>
     </row>
     <row r="216" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A216" s="4" t="s">
-        <v>2367</v>
+        <v>2371</v>
       </c>
     </row>
     <row r="217" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A217" s="4" t="s">
-        <v>2368</v>
+        <v>2372</v>
       </c>
     </row>
     <row r="218" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A218" s="4" t="s">
-        <v>2369</v>
+        <v>2373</v>
       </c>
     </row>
     <row r="219" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A219" s="4" t="s">
-        <v>2371</v>
+        <v>2375</v>
       </c>
     </row>
     <row r="220" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A220" s="4" t="s">
-        <v>2372</v>
+        <v>2376</v>
       </c>
     </row>
     <row r="221" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A221" s="4" t="s">
-        <v>2373</v>
+        <v>2377</v>
       </c>
     </row>
     <row r="222" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A222" s="4" t="s">
-        <v>2375</v>
+        <v>2379</v>
       </c>
     </row>
     <row r="223" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A223" s="4" t="s">
-        <v>2376</v>
+        <v>2380</v>
       </c>
     </row>
     <row r="224" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A224" s="4" t="s">
-        <v>2377</v>
+        <v>2381</v>
       </c>
     </row>
     <row r="225" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A225" s="4" t="s">
-        <v>2379</v>
+        <v>2383</v>
       </c>
     </row>
     <row r="226" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A226" s="4" t="s">
-        <v>2380</v>
+        <v>2384</v>
       </c>
     </row>
     <row r="227" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A227" s="4" t="s">
-        <v>2381</v>
+        <v>2385</v>
       </c>
     </row>
     <row r="228" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A228" s="4" t="s">
-        <v>2383</v>
+        <v>2387</v>
       </c>
     </row>
     <row r="229" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A229" s="4" t="s">
-        <v>2384</v>
+        <v>2388</v>
       </c>
     </row>
     <row r="230" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A230" s="4" t="s">
-        <v>2385</v>
+        <v>2389</v>
       </c>
     </row>
     <row r="231" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A231" s="4" t="s">
-        <v>2387</v>
+        <v>2391</v>
       </c>
     </row>
     <row r="232" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A232" s="4" t="s">
-        <v>2388</v>
+        <v>2392</v>
       </c>
     </row>
     <row r="233" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A233" s="4" t="s">
-        <v>2389</v>
+        <v>2393</v>
       </c>
     </row>
     <row r="234" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A234" s="4" t="s">
-        <v>2391</v>
+        <v>2395</v>
       </c>
     </row>
     <row r="235" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A235" s="4" t="s">
-        <v>2392</v>
+        <v>2396</v>
       </c>
     </row>
     <row r="236" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A236" s="4" t="s">
-        <v>2393</v>
+        <v>2397</v>
       </c>
     </row>
     <row r="237" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A237" s="4" t="s">
-        <v>2395</v>
+        <v>2399</v>
       </c>
     </row>
     <row r="238" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A238" s="4" t="s">
-        <v>2396</v>
+        <v>2400</v>
       </c>
     </row>
     <row r="239" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A239" s="4" t="s">
-        <v>2397</v>
+        <v>2402</v>
       </c>
     </row>
     <row r="240" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A240" s="4" t="s">
-        <v>2399</v>
+        <v>2403</v>
       </c>
     </row>
     <row r="241" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A241" s="4" t="s">
-        <v>2400</v>
+        <v>2404</v>
       </c>
     </row>
     <row r="242" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A242" s="4" t="s">
-        <v>2402</v>
+        <v>2406</v>
       </c>
     </row>
     <row r="243" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A243" s="4" t="s">
-        <v>2403</v>
+        <v>2407</v>
       </c>
     </row>
     <row r="244" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A244" s="4" t="s">
-        <v>2404</v>
+        <v>2408</v>
       </c>
     </row>
     <row r="245" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A245" s="4" t="s">
-        <v>2406</v>
+        <v>2410</v>
       </c>
     </row>
     <row r="246" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A246" s="4" t="s">
-        <v>2407</v>
+        <v>2411</v>
       </c>
     </row>
     <row r="247" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A247" s="4" t="s">
-        <v>2408</v>
+        <v>2412</v>
       </c>
     </row>
     <row r="248" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A248" s="4" t="s">
-        <v>2410</v>
+        <v>2414</v>
       </c>
     </row>
     <row r="249" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A249" s="4" t="s">
-        <v>2411</v>
+        <v>2415</v>
       </c>
     </row>
     <row r="250" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A250" s="4" t="s">
-        <v>2412</v>
+        <v>2416</v>
       </c>
     </row>
     <row r="251" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A251" s="4" t="s">
-        <v>2414</v>
+        <v>2418</v>
       </c>
     </row>
     <row r="252" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A252" s="4" t="s">
-        <v>2415</v>
+        <v>2419</v>
       </c>
     </row>
     <row r="253" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A253" s="4" t="s">
-        <v>2416</v>
+        <v>2420</v>
       </c>
     </row>
     <row r="254" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A254" s="4" t="s">
-        <v>2418</v>
+        <v>2422</v>
       </c>
     </row>
     <row r="255" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A255" s="4" t="s">
-        <v>2419</v>
+        <v>2423</v>
       </c>
     </row>
     <row r="256" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A256" s="4" t="s">
-        <v>2420</v>
+        <v>2424</v>
       </c>
     </row>
     <row r="257" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A257" s="4" t="s">
-        <v>2422</v>
+        <v>2426</v>
       </c>
     </row>
     <row r="258" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A258" s="4" t="s">
-        <v>2423</v>
+        <v>2427</v>
       </c>
     </row>
     <row r="259" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A259" s="4" t="s">
-        <v>2424</v>
+        <v>2428</v>
       </c>
     </row>
     <row r="260" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A260" s="4" t="s">
-        <v>2426</v>
+        <v>2430</v>
       </c>
     </row>
     <row r="261" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A261" s="4" t="s">
-        <v>2427</v>
+        <v>2431</v>
       </c>
     </row>
     <row r="262" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A262" s="4" t="s">
-        <v>2428</v>
+        <v>2432</v>
       </c>
     </row>
     <row r="263" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A263" s="4" t="s">
-        <v>2430</v>
+        <v>2434</v>
       </c>
     </row>
     <row r="264" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A264" s="4" t="s">
-        <v>2431</v>
+        <v>2435</v>
       </c>
     </row>
     <row r="265" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A265" s="4" t="s">
-        <v>2432</v>
+        <v>2437</v>
       </c>
     </row>
     <row r="266" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A266" s="4" t="s">
-        <v>2434</v>
+        <v>2438</v>
       </c>
     </row>
     <row r="267" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A267" s="4" t="s">
-        <v>2435</v>
-      </c>
-    </row>
-    <row r="268" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A268" s="4" t="s">
-        <v>2437</v>
-      </c>
-    </row>
-    <row r="269" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A269" s="4" t="s">
-        <v>2438</v>
-      </c>
-    </row>
-    <row r="270" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A270" s="4" t="s">
         <v>2439</v>
       </c>
     </row>
@@ -19338,158 +18375,155 @@
     <hyperlink ref="A122" r:id="rId122" xr:uid="{DD6F696E-AEFA-7D43-B9A3-FA00CAFFDC6F}"/>
     <hyperlink ref="A123" r:id="rId123" xr:uid="{8D9ABDD9-8D5D-634F-A99E-C5682B376EF5}"/>
     <hyperlink ref="A124" r:id="rId124" xr:uid="{3656A3AD-32C7-D94E-A003-F0349E3FEDF7}"/>
-    <hyperlink ref="A125" r:id="rId125" xr:uid="{8CD08AD2-D2A8-0848-96E7-7E04E09A9DD1}"/>
-    <hyperlink ref="A126" r:id="rId126" xr:uid="{9A4B6EDA-774B-B54D-A914-4147FBEBE5E0}"/>
-    <hyperlink ref="A127" r:id="rId127" xr:uid="{8D796A46-86DF-934D-A2CA-5FFE9DF94682}"/>
-    <hyperlink ref="A128" r:id="rId128" xr:uid="{43CF84D5-0469-E343-9994-8169CA64BA9C}"/>
-    <hyperlink ref="A129" r:id="rId129" xr:uid="{C23D1F80-C381-B841-A8A1-2CC5DFD5F3D3}"/>
-    <hyperlink ref="A130" r:id="rId130" xr:uid="{2444B9A3-8449-C946-B3B5-E4C6AF7AE7D6}"/>
-    <hyperlink ref="A131" r:id="rId131" xr:uid="{64A57281-30DB-6246-BF27-C712C5CA5EBE}"/>
-    <hyperlink ref="A132" r:id="rId132" xr:uid="{4A2EB155-A84C-C54B-8674-3C8E49A2EA67}"/>
-    <hyperlink ref="A133" r:id="rId133" xr:uid="{4CE353F6-480F-9540-B15F-BDD2783FFF2B}"/>
-    <hyperlink ref="A134" r:id="rId134" xr:uid="{CBF3C27E-1826-954D-8E48-9B5BCFA31E08}"/>
-    <hyperlink ref="A135" r:id="rId135" xr:uid="{4C5C94DE-32E1-1C41-ADB8-A2FBF71143F9}"/>
-    <hyperlink ref="A136" r:id="rId136" xr:uid="{ED77BB1A-9E08-EB45-B147-A10D0651FB6E}"/>
-    <hyperlink ref="A137" r:id="rId137" xr:uid="{871748FF-4C47-2943-8C64-4948D2E61E68}"/>
-    <hyperlink ref="A138" r:id="rId138" xr:uid="{CD9A6AA8-19BB-0040-BD96-DE5B25952538}"/>
-    <hyperlink ref="A139" r:id="rId139" xr:uid="{7CD1970F-CF55-B94F-AA51-D32511853502}"/>
-    <hyperlink ref="A140" r:id="rId140" xr:uid="{5B3D19A9-8B6F-CB4C-9AB3-7558BAFE2B25}"/>
-    <hyperlink ref="A141" r:id="rId141" xr:uid="{EF1DD75B-A11C-D24A-82AF-63FB93408CEA}"/>
-    <hyperlink ref="A142" r:id="rId142" xr:uid="{B1CED060-AA86-A543-AB67-6E553660DCF0}"/>
-    <hyperlink ref="A143" r:id="rId143" xr:uid="{FE1CD0E2-C168-CE47-B4A5-17FD60A0E8A6}"/>
-    <hyperlink ref="A144" r:id="rId144" xr:uid="{E151DCAA-D54A-A34F-8492-6FD5A4E110EB}"/>
-    <hyperlink ref="A145" r:id="rId145" xr:uid="{4BF4BFFB-BFA1-4C42-9CB7-6EF724667CD3}"/>
-    <hyperlink ref="A146" r:id="rId146" xr:uid="{B27D089C-15F3-4E40-93C7-43587D260AA1}"/>
-    <hyperlink ref="A147" r:id="rId147" xr:uid="{13075B7B-425E-DB41-BD0E-A9AFA888A2C1}"/>
-    <hyperlink ref="A148" r:id="rId148" xr:uid="{90A365BA-1B76-D449-9956-A7FF38CA7E97}"/>
-    <hyperlink ref="A149" r:id="rId149" xr:uid="{545A4385-6EEE-614E-A094-C51E3469E7F6}"/>
-    <hyperlink ref="A150" r:id="rId150" xr:uid="{D4B43F7F-A8FB-F542-8701-59A373109D6E}"/>
-    <hyperlink ref="A151" r:id="rId151" xr:uid="{E6F8BE0B-5173-8F46-9977-08C49FC198CC}"/>
-    <hyperlink ref="A152" r:id="rId152" xr:uid="{8B965D12-34F6-454C-8DEB-484048172E66}"/>
-    <hyperlink ref="A153" r:id="rId153" xr:uid="{B6823E5C-0B1D-0B40-913A-53609E9575FE}"/>
-    <hyperlink ref="A154" r:id="rId154" xr:uid="{1DE0650F-86B7-F845-A8EC-50037A436127}"/>
-    <hyperlink ref="A155" r:id="rId155" xr:uid="{8883F87B-B7E8-3442-AC0E-78E5E482FEB2}"/>
-    <hyperlink ref="A156" r:id="rId156" xr:uid="{A2572AA2-848B-2745-8C3B-5CC205D19641}"/>
-    <hyperlink ref="A157" r:id="rId157" xr:uid="{6C6744D9-B8E9-2C4C-8589-196C6BF2D5E5}"/>
-    <hyperlink ref="A158" r:id="rId158" xr:uid="{DCBE8BC1-4696-144C-AC99-90FBBB80F45E}"/>
-    <hyperlink ref="A159" r:id="rId159" xr:uid="{CEC05240-2382-B54B-9AD7-FE27655139F9}"/>
-    <hyperlink ref="A160" r:id="rId160" xr:uid="{A5251266-5D55-2544-94F4-EA3DAD18B30E}"/>
-    <hyperlink ref="A161" r:id="rId161" xr:uid="{C0104702-E7D1-7846-869D-6D60E906D907}"/>
-    <hyperlink ref="A162" r:id="rId162" xr:uid="{561BE00D-F7D8-FC49-8444-FEBC64764FD9}"/>
-    <hyperlink ref="A163" r:id="rId163" xr:uid="{AA02CAE1-75D9-3E42-B30F-A634B26A998D}"/>
-    <hyperlink ref="A164" r:id="rId164" xr:uid="{B79A3596-90E1-3348-9D6D-0A2146F5C97F}"/>
-    <hyperlink ref="A165" r:id="rId165" xr:uid="{6CB03193-7301-BD46-A8BE-F6F8FF9FD1F2}"/>
-    <hyperlink ref="A166" r:id="rId166" xr:uid="{26FF1C0C-88B4-2444-9DE1-BDA93BE0DC21}"/>
-    <hyperlink ref="A167" r:id="rId167" xr:uid="{1261B7AD-6EEF-FA45-8A4A-A4F17D2B8421}"/>
-    <hyperlink ref="A168" r:id="rId168" xr:uid="{234E8BAE-E68B-474E-9885-368948912457}"/>
-    <hyperlink ref="A169" r:id="rId169" xr:uid="{D4945377-E48E-D54B-97EC-C3A4B303EA5A}"/>
-    <hyperlink ref="A170" r:id="rId170" xr:uid="{53F054A4-681E-2F4B-B62C-E797DD9742F1}"/>
-    <hyperlink ref="A171" r:id="rId171" xr:uid="{5FF0CE08-BEA7-9B47-9CB9-D79E463EE67D}"/>
-    <hyperlink ref="A172" r:id="rId172" xr:uid="{9C41982C-30C0-E44F-94C7-41C5F6C667F2}"/>
-    <hyperlink ref="A173" r:id="rId173" xr:uid="{45CDA606-3E25-5246-B064-83CB1CE897F9}"/>
-    <hyperlink ref="A174" r:id="rId174" xr:uid="{66B8D53F-BA43-C34D-850C-89C9BA6CBF3A}"/>
-    <hyperlink ref="A175" r:id="rId175" xr:uid="{E70D5015-68CA-F745-B6A3-718A3AED4C3F}"/>
-    <hyperlink ref="A176" r:id="rId176" xr:uid="{143A5153-9C90-4C4A-98D6-377A7C7823E6}"/>
-    <hyperlink ref="A177" r:id="rId177" xr:uid="{377A593A-66AE-B147-AD6F-FC2424F6C722}"/>
-    <hyperlink ref="A178" r:id="rId178" xr:uid="{DE5F3D95-9B10-4C4F-ACB6-00D167CE8BD3}"/>
-    <hyperlink ref="A179" r:id="rId179" xr:uid="{DC857D2D-3097-944D-A1F1-2E9CA1940F2E}"/>
-    <hyperlink ref="A180" r:id="rId180" xr:uid="{38CE3C9D-3195-A344-BE56-C80904E459D9}"/>
-    <hyperlink ref="A181" r:id="rId181" xr:uid="{1F265E26-E372-F545-9586-95D236A44422}"/>
-    <hyperlink ref="A182" r:id="rId182" xr:uid="{02B00F99-7259-9549-966A-DBCA6774A5A1}"/>
-    <hyperlink ref="A183" r:id="rId183" xr:uid="{6C996963-BBF1-9D4B-9524-5ECA8AA86ABD}"/>
-    <hyperlink ref="A184" r:id="rId184" xr:uid="{C7709FEC-E79F-904F-83BA-B5B2D8BFB797}"/>
-    <hyperlink ref="A185" r:id="rId185" xr:uid="{4E99D51F-EB29-6141-B00D-10D0D68D5664}"/>
-    <hyperlink ref="A186" r:id="rId186" xr:uid="{6F9C07D2-4213-6D4D-8A4D-EE30DCDDB085}"/>
-    <hyperlink ref="A187" r:id="rId187" xr:uid="{02BD1FD6-85EC-304D-A3EF-912223B3D3B9}"/>
-    <hyperlink ref="A188" r:id="rId188" xr:uid="{FA0A6533-4D97-7A41-9D6B-6F42FA8B278B}"/>
-    <hyperlink ref="A189" r:id="rId189" xr:uid="{A26B9C32-14F4-8947-9103-5150C02831D7}"/>
-    <hyperlink ref="A190" r:id="rId190" xr:uid="{AE125B6A-6B49-7C4A-96E9-B6617E97CCC9}"/>
-    <hyperlink ref="A191" r:id="rId191" xr:uid="{B7C8C160-062F-CF49-B79C-49AE862E384F}"/>
-    <hyperlink ref="A192" r:id="rId192" xr:uid="{864905D7-5DD3-834B-B0D2-8E99D9ACE1CE}"/>
-    <hyperlink ref="A193" r:id="rId193" xr:uid="{A4208BFB-EEC0-9D42-B701-5168FA0E70B6}"/>
-    <hyperlink ref="A194" r:id="rId194" xr:uid="{A8548243-D6E3-9345-9F1E-60D9BE73D3AF}"/>
-    <hyperlink ref="A195" r:id="rId195" xr:uid="{E39BF1B3-D42A-0B44-83A7-C6B99B9432F0}"/>
-    <hyperlink ref="A196" r:id="rId196" xr:uid="{86807DD1-A847-4146-8A1F-3553FA25999E}"/>
-    <hyperlink ref="A197" r:id="rId197" xr:uid="{23574F31-648E-4344-8386-120463AA41C3}"/>
-    <hyperlink ref="A198" r:id="rId198" xr:uid="{B662A1B6-DB71-7543-B0C3-EDAEB5E898EA}"/>
-    <hyperlink ref="A199" r:id="rId199" xr:uid="{6F283435-2B29-3E48-BAD7-09C8EFA778C0}"/>
-    <hyperlink ref="A200" r:id="rId200" xr:uid="{64E28DAD-D20E-6A4A-B791-C2C5F61C97F7}"/>
-    <hyperlink ref="A201" r:id="rId201" xr:uid="{D2192D39-8FE4-294B-9BAA-6354AAF827C1}"/>
-    <hyperlink ref="A202" r:id="rId202" xr:uid="{026FD04C-DFFE-7446-BE19-7C692A5E7D45}"/>
-    <hyperlink ref="A203" r:id="rId203" xr:uid="{4B6827E9-5133-534F-A378-33B74C97B9E8}"/>
-    <hyperlink ref="A204" r:id="rId204" xr:uid="{905A9DFC-542E-3746-88AA-0613D26AEB4A}"/>
-    <hyperlink ref="A205" r:id="rId205" xr:uid="{6E0FAD1E-85C8-7E4D-999F-2443AC337F49}"/>
-    <hyperlink ref="A206" r:id="rId206" xr:uid="{94C5E53C-083C-8245-A3C0-DC78DF88F801}"/>
-    <hyperlink ref="A207" r:id="rId207" xr:uid="{C607D1D1-522F-A740-B5FE-C79E1B520964}"/>
-    <hyperlink ref="A208" r:id="rId208" xr:uid="{73B203FD-ABFE-004D-B61F-5481BBA0AB32}"/>
-    <hyperlink ref="A209" r:id="rId209" xr:uid="{8D2BC35C-0804-014C-8B5D-68D074DF97CE}"/>
-    <hyperlink ref="A210" r:id="rId210" xr:uid="{37880A7A-2513-6E44-BEC8-26F48632CFE2}"/>
-    <hyperlink ref="A211" r:id="rId211" xr:uid="{01CB8167-73D3-024D-97E8-7B9825772262}"/>
-    <hyperlink ref="A212" r:id="rId212" xr:uid="{D44C03AC-C3B4-3E4E-996A-AD53674D61AD}"/>
-    <hyperlink ref="A213" r:id="rId213" xr:uid="{25B5C679-739F-5242-B526-6BEA2ABCC9B4}"/>
-    <hyperlink ref="A214" r:id="rId214" xr:uid="{272862B1-AB15-064B-A4EF-D92DBCFFC594}"/>
-    <hyperlink ref="A215" r:id="rId215" xr:uid="{5E8D8D9E-D52D-354A-A4E9-227F493A2F3C}"/>
-    <hyperlink ref="A216" r:id="rId216" xr:uid="{43CD4AFC-0A4B-604A-9B63-432C8B184388}"/>
-    <hyperlink ref="A217" r:id="rId217" xr:uid="{C797B4FD-256C-7B47-8ABE-51742284D7C1}"/>
-    <hyperlink ref="A218" r:id="rId218" xr:uid="{9D43C380-B61B-0E45-9EFE-22F3D589228F}"/>
-    <hyperlink ref="A219" r:id="rId219" xr:uid="{5BF51224-D2D2-4E4F-94A8-0E264DBAE644}"/>
-    <hyperlink ref="A220" r:id="rId220" xr:uid="{0C5F26D2-9FCE-544D-BFCE-43E9E9B53798}"/>
-    <hyperlink ref="A221" r:id="rId221" xr:uid="{3DFD6606-C5E0-1947-A1B4-45FB0DDB2DEF}"/>
-    <hyperlink ref="A222" r:id="rId222" xr:uid="{008C6F3E-FC65-0C4C-A8E0-73CF59234684}"/>
-    <hyperlink ref="A223" r:id="rId223" xr:uid="{DF0FEFC5-427A-C047-ACD4-6C21318E1E23}"/>
-    <hyperlink ref="A224" r:id="rId224" xr:uid="{92AF8662-902C-804E-9030-0BAB9813C845}"/>
-    <hyperlink ref="A225" r:id="rId225" xr:uid="{71B613A7-0D55-7145-AC5B-02FD3BE2CAB8}"/>
-    <hyperlink ref="A226" r:id="rId226" xr:uid="{2CF44E20-9FFA-4B43-89C9-6E9FA6B19B52}"/>
-    <hyperlink ref="A227" r:id="rId227" xr:uid="{DB17333E-F6FC-FC49-B299-92058B80A305}"/>
-    <hyperlink ref="A228" r:id="rId228" xr:uid="{3CEFC6FF-932F-A24D-BF78-807549577A1C}"/>
-    <hyperlink ref="A229" r:id="rId229" xr:uid="{46BDDC05-1A90-B74E-A977-576480262C92}"/>
-    <hyperlink ref="A230" r:id="rId230" xr:uid="{738AEE97-2EE2-534E-8DDE-4341C066C6B6}"/>
-    <hyperlink ref="A231" r:id="rId231" xr:uid="{E7523842-A33A-DC45-8CCE-4066F5FB1B27}"/>
-    <hyperlink ref="A232" r:id="rId232" xr:uid="{79E590E7-0A9A-5841-9516-CCD47B597BF8}"/>
-    <hyperlink ref="A233" r:id="rId233" xr:uid="{7588C0D6-F57E-DD4E-AC90-724B07456150}"/>
-    <hyperlink ref="A234" r:id="rId234" xr:uid="{DE6D27E1-64D6-D842-AB75-774DE8229957}"/>
-    <hyperlink ref="A235" r:id="rId235" xr:uid="{01AF2C8D-352D-314A-8D6F-3B67A4C8C51E}"/>
-    <hyperlink ref="A236" r:id="rId236" xr:uid="{B117BD27-D7DB-7D45-9E62-17C0022E0C30}"/>
-    <hyperlink ref="A237" r:id="rId237" xr:uid="{7E805266-54F3-8D4B-96E6-DE90B976271C}"/>
-    <hyperlink ref="A238" r:id="rId238" xr:uid="{7FECA922-803E-B541-BD70-C92210259589}"/>
-    <hyperlink ref="A239" r:id="rId239" xr:uid="{A06C925D-130A-2C45-9FFA-E5ED62BCF903}"/>
-    <hyperlink ref="A240" r:id="rId240" xr:uid="{86952E20-34E4-BE4C-9B7E-05AE96D67C49}"/>
-    <hyperlink ref="A241" r:id="rId241" xr:uid="{428714E7-1F49-5E47-A7B4-FBB5FBE5B677}"/>
-    <hyperlink ref="A242" r:id="rId242" xr:uid="{CDCE6BC6-FEA9-E24F-97A1-BA6DAF9F3689}"/>
-    <hyperlink ref="A243" r:id="rId243" xr:uid="{9A51FAA8-CAF9-EB49-B871-9B7288385456}"/>
-    <hyperlink ref="A244" r:id="rId244" xr:uid="{5C9784D1-0EEF-5042-916F-E27F3BB19F64}"/>
-    <hyperlink ref="A245" r:id="rId245" xr:uid="{D4D8E38F-8C88-5A4F-8C1A-65B2122054A8}"/>
-    <hyperlink ref="A246" r:id="rId246" xr:uid="{921F652B-C654-EE43-928D-3E9B698DE534}"/>
-    <hyperlink ref="A247" r:id="rId247" xr:uid="{DE0AAE01-548C-7A4E-8C00-7F53FFB019F1}"/>
-    <hyperlink ref="A248" r:id="rId248" xr:uid="{66321B79-3291-6744-B4F3-AA7875F908CD}"/>
-    <hyperlink ref="A249" r:id="rId249" xr:uid="{C1F12D44-80AA-2B4A-9918-ABD7B564E6D1}"/>
-    <hyperlink ref="A250" r:id="rId250" xr:uid="{CFBA8119-5235-3547-A11B-DE68DC150A56}"/>
-    <hyperlink ref="A251" r:id="rId251" xr:uid="{6586FC0D-D311-8F47-A84E-82044CA7AF00}"/>
-    <hyperlink ref="A252" r:id="rId252" xr:uid="{5168A552-E3CB-AC40-AB67-25F57D51FADC}"/>
-    <hyperlink ref="A253" r:id="rId253" xr:uid="{5EFEAE08-0D33-3540-A0B7-4080163E0257}"/>
-    <hyperlink ref="A254" r:id="rId254" xr:uid="{8B9E93C8-0330-9944-9569-068E818AC275}"/>
-    <hyperlink ref="A255" r:id="rId255" xr:uid="{8FE95D37-BEBC-F645-8547-C28857B0A45C}"/>
-    <hyperlink ref="A256" r:id="rId256" xr:uid="{D89CCFEC-D0A3-8B48-8AD9-B1DBBC58B978}"/>
-    <hyperlink ref="A257" r:id="rId257" xr:uid="{8EFFFD9C-30C7-4048-9576-B9744E0AAA6D}"/>
-    <hyperlink ref="A258" r:id="rId258" xr:uid="{6A1239DA-4F6F-324B-8406-E5968BF79193}"/>
-    <hyperlink ref="A259" r:id="rId259" xr:uid="{1FB0358F-8137-E346-8B37-A88DA58FF893}"/>
-    <hyperlink ref="A260" r:id="rId260" xr:uid="{7393D797-F331-2747-B21F-9C64477B03E8}"/>
-    <hyperlink ref="A261" r:id="rId261" xr:uid="{89241C78-8C33-8A4B-9191-27ABCFD624DD}"/>
-    <hyperlink ref="A262" r:id="rId262" xr:uid="{58611FFD-E629-A44B-8459-DBE392F39DDE}"/>
-    <hyperlink ref="A263" r:id="rId263" xr:uid="{FC27C60A-E408-804E-855C-1CBA151805E0}"/>
-    <hyperlink ref="A264" r:id="rId264" xr:uid="{31CA7AA2-EF5D-DA44-B167-D56CD35E223C}"/>
-    <hyperlink ref="A265" r:id="rId265" xr:uid="{DDC1BD5A-FC66-FB42-B1CB-034865EC2803}"/>
-    <hyperlink ref="A266" r:id="rId266" xr:uid="{8BD644BD-BAF3-7544-860E-00515810E7AE}"/>
-    <hyperlink ref="A267" r:id="rId267" xr:uid="{55FC32CC-5C56-4E43-99E9-7FCFD2E9E866}"/>
-    <hyperlink ref="A268" r:id="rId268" xr:uid="{9F390145-95BE-1D41-8C2C-241EBBE828EF}"/>
-    <hyperlink ref="A269" r:id="rId269" xr:uid="{05530643-B829-EE42-81CA-23F84CE6A2EF}"/>
-    <hyperlink ref="A270" r:id="rId270" xr:uid="{28D44972-71E5-D642-A427-2F69E1E61BB5}"/>
+    <hyperlink ref="A125" r:id="rId125" xr:uid="{43CF84D5-0469-E343-9994-8169CA64BA9C}"/>
+    <hyperlink ref="A126" r:id="rId126" xr:uid="{C23D1F80-C381-B841-A8A1-2CC5DFD5F3D3}"/>
+    <hyperlink ref="A127" r:id="rId127" xr:uid="{2444B9A3-8449-C946-B3B5-E4C6AF7AE7D6}"/>
+    <hyperlink ref="A128" r:id="rId128" xr:uid="{64A57281-30DB-6246-BF27-C712C5CA5EBE}"/>
+    <hyperlink ref="A129" r:id="rId129" xr:uid="{4A2EB155-A84C-C54B-8674-3C8E49A2EA67}"/>
+    <hyperlink ref="A130" r:id="rId130" xr:uid="{4CE353F6-480F-9540-B15F-BDD2783FFF2B}"/>
+    <hyperlink ref="A131" r:id="rId131" xr:uid="{CBF3C27E-1826-954D-8E48-9B5BCFA31E08}"/>
+    <hyperlink ref="A132" r:id="rId132" xr:uid="{4C5C94DE-32E1-1C41-ADB8-A2FBF71143F9}"/>
+    <hyperlink ref="A133" r:id="rId133" xr:uid="{ED77BB1A-9E08-EB45-B147-A10D0651FB6E}"/>
+    <hyperlink ref="A134" r:id="rId134" xr:uid="{871748FF-4C47-2943-8C64-4948D2E61E68}"/>
+    <hyperlink ref="A135" r:id="rId135" xr:uid="{CD9A6AA8-19BB-0040-BD96-DE5B25952538}"/>
+    <hyperlink ref="A136" r:id="rId136" xr:uid="{7CD1970F-CF55-B94F-AA51-D32511853502}"/>
+    <hyperlink ref="A137" r:id="rId137" xr:uid="{5B3D19A9-8B6F-CB4C-9AB3-7558BAFE2B25}"/>
+    <hyperlink ref="A138" r:id="rId138" xr:uid="{EF1DD75B-A11C-D24A-82AF-63FB93408CEA}"/>
+    <hyperlink ref="A139" r:id="rId139" xr:uid="{B1CED060-AA86-A543-AB67-6E553660DCF0}"/>
+    <hyperlink ref="A140" r:id="rId140" xr:uid="{FE1CD0E2-C168-CE47-B4A5-17FD60A0E8A6}"/>
+    <hyperlink ref="A141" r:id="rId141" xr:uid="{E151DCAA-D54A-A34F-8492-6FD5A4E110EB}"/>
+    <hyperlink ref="A142" r:id="rId142" xr:uid="{4BF4BFFB-BFA1-4C42-9CB7-6EF724667CD3}"/>
+    <hyperlink ref="A143" r:id="rId143" xr:uid="{B27D089C-15F3-4E40-93C7-43587D260AA1}"/>
+    <hyperlink ref="A144" r:id="rId144" xr:uid="{13075B7B-425E-DB41-BD0E-A9AFA888A2C1}"/>
+    <hyperlink ref="A145" r:id="rId145" xr:uid="{90A365BA-1B76-D449-9956-A7FF38CA7E97}"/>
+    <hyperlink ref="A146" r:id="rId146" xr:uid="{545A4385-6EEE-614E-A094-C51E3469E7F6}"/>
+    <hyperlink ref="A147" r:id="rId147" xr:uid="{D4B43F7F-A8FB-F542-8701-59A373109D6E}"/>
+    <hyperlink ref="A148" r:id="rId148" xr:uid="{E6F8BE0B-5173-8F46-9977-08C49FC198CC}"/>
+    <hyperlink ref="A149" r:id="rId149" xr:uid="{8B965D12-34F6-454C-8DEB-484048172E66}"/>
+    <hyperlink ref="A150" r:id="rId150" xr:uid="{B6823E5C-0B1D-0B40-913A-53609E9575FE}"/>
+    <hyperlink ref="A151" r:id="rId151" xr:uid="{1DE0650F-86B7-F845-A8EC-50037A436127}"/>
+    <hyperlink ref="A152" r:id="rId152" xr:uid="{8883F87B-B7E8-3442-AC0E-78E5E482FEB2}"/>
+    <hyperlink ref="A153" r:id="rId153" xr:uid="{A2572AA2-848B-2745-8C3B-5CC205D19641}"/>
+    <hyperlink ref="A154" r:id="rId154" xr:uid="{6C6744D9-B8E9-2C4C-8589-196C6BF2D5E5}"/>
+    <hyperlink ref="A155" r:id="rId155" xr:uid="{DCBE8BC1-4696-144C-AC99-90FBBB80F45E}"/>
+    <hyperlink ref="A156" r:id="rId156" xr:uid="{CEC05240-2382-B54B-9AD7-FE27655139F9}"/>
+    <hyperlink ref="A157" r:id="rId157" xr:uid="{A5251266-5D55-2544-94F4-EA3DAD18B30E}"/>
+    <hyperlink ref="A158" r:id="rId158" xr:uid="{C0104702-E7D1-7846-869D-6D60E906D907}"/>
+    <hyperlink ref="A159" r:id="rId159" xr:uid="{561BE00D-F7D8-FC49-8444-FEBC64764FD9}"/>
+    <hyperlink ref="A160" r:id="rId160" xr:uid="{AA02CAE1-75D9-3E42-B30F-A634B26A998D}"/>
+    <hyperlink ref="A161" r:id="rId161" xr:uid="{B79A3596-90E1-3348-9D6D-0A2146F5C97F}"/>
+    <hyperlink ref="A162" r:id="rId162" xr:uid="{6CB03193-7301-BD46-A8BE-F6F8FF9FD1F2}"/>
+    <hyperlink ref="A163" r:id="rId163" xr:uid="{26FF1C0C-88B4-2444-9DE1-BDA93BE0DC21}"/>
+    <hyperlink ref="A164" r:id="rId164" xr:uid="{1261B7AD-6EEF-FA45-8A4A-A4F17D2B8421}"/>
+    <hyperlink ref="A165" r:id="rId165" xr:uid="{234E8BAE-E68B-474E-9885-368948912457}"/>
+    <hyperlink ref="A166" r:id="rId166" xr:uid="{D4945377-E48E-D54B-97EC-C3A4B303EA5A}"/>
+    <hyperlink ref="A167" r:id="rId167" xr:uid="{53F054A4-681E-2F4B-B62C-E797DD9742F1}"/>
+    <hyperlink ref="A168" r:id="rId168" xr:uid="{5FF0CE08-BEA7-9B47-9CB9-D79E463EE67D}"/>
+    <hyperlink ref="A169" r:id="rId169" xr:uid="{9C41982C-30C0-E44F-94C7-41C5F6C667F2}"/>
+    <hyperlink ref="A170" r:id="rId170" xr:uid="{45CDA606-3E25-5246-B064-83CB1CE897F9}"/>
+    <hyperlink ref="A171" r:id="rId171" xr:uid="{66B8D53F-BA43-C34D-850C-89C9BA6CBF3A}"/>
+    <hyperlink ref="A172" r:id="rId172" xr:uid="{E70D5015-68CA-F745-B6A3-718A3AED4C3F}"/>
+    <hyperlink ref="A173" r:id="rId173" xr:uid="{143A5153-9C90-4C4A-98D6-377A7C7823E6}"/>
+    <hyperlink ref="A174" r:id="rId174" xr:uid="{377A593A-66AE-B147-AD6F-FC2424F6C722}"/>
+    <hyperlink ref="A175" r:id="rId175" xr:uid="{DE5F3D95-9B10-4C4F-ACB6-00D167CE8BD3}"/>
+    <hyperlink ref="A176" r:id="rId176" xr:uid="{DC857D2D-3097-944D-A1F1-2E9CA1940F2E}"/>
+    <hyperlink ref="A177" r:id="rId177" xr:uid="{38CE3C9D-3195-A344-BE56-C80904E459D9}"/>
+    <hyperlink ref="A178" r:id="rId178" xr:uid="{1F265E26-E372-F545-9586-95D236A44422}"/>
+    <hyperlink ref="A179" r:id="rId179" xr:uid="{02B00F99-7259-9549-966A-DBCA6774A5A1}"/>
+    <hyperlink ref="A180" r:id="rId180" xr:uid="{6C996963-BBF1-9D4B-9524-5ECA8AA86ABD}"/>
+    <hyperlink ref="A181" r:id="rId181" xr:uid="{C7709FEC-E79F-904F-83BA-B5B2D8BFB797}"/>
+    <hyperlink ref="A182" r:id="rId182" xr:uid="{4E99D51F-EB29-6141-B00D-10D0D68D5664}"/>
+    <hyperlink ref="A183" r:id="rId183" xr:uid="{6F9C07D2-4213-6D4D-8A4D-EE30DCDDB085}"/>
+    <hyperlink ref="A184" r:id="rId184" xr:uid="{02BD1FD6-85EC-304D-A3EF-912223B3D3B9}"/>
+    <hyperlink ref="A185" r:id="rId185" xr:uid="{FA0A6533-4D97-7A41-9D6B-6F42FA8B278B}"/>
+    <hyperlink ref="A186" r:id="rId186" xr:uid="{A26B9C32-14F4-8947-9103-5150C02831D7}"/>
+    <hyperlink ref="A187" r:id="rId187" xr:uid="{AE125B6A-6B49-7C4A-96E9-B6617E97CCC9}"/>
+    <hyperlink ref="A188" r:id="rId188" xr:uid="{B7C8C160-062F-CF49-B79C-49AE862E384F}"/>
+    <hyperlink ref="A189" r:id="rId189" xr:uid="{864905D7-5DD3-834B-B0D2-8E99D9ACE1CE}"/>
+    <hyperlink ref="A190" r:id="rId190" xr:uid="{A4208BFB-EEC0-9D42-B701-5168FA0E70B6}"/>
+    <hyperlink ref="A191" r:id="rId191" xr:uid="{A8548243-D6E3-9345-9F1E-60D9BE73D3AF}"/>
+    <hyperlink ref="A192" r:id="rId192" xr:uid="{E39BF1B3-D42A-0B44-83A7-C6B99B9432F0}"/>
+    <hyperlink ref="A193" r:id="rId193" xr:uid="{86807DD1-A847-4146-8A1F-3553FA25999E}"/>
+    <hyperlink ref="A194" r:id="rId194" xr:uid="{23574F31-648E-4344-8386-120463AA41C3}"/>
+    <hyperlink ref="A195" r:id="rId195" xr:uid="{B662A1B6-DB71-7543-B0C3-EDAEB5E898EA}"/>
+    <hyperlink ref="A196" r:id="rId196" xr:uid="{6F283435-2B29-3E48-BAD7-09C8EFA778C0}"/>
+    <hyperlink ref="A197" r:id="rId197" xr:uid="{64E28DAD-D20E-6A4A-B791-C2C5F61C97F7}"/>
+    <hyperlink ref="A198" r:id="rId198" xr:uid="{D2192D39-8FE4-294B-9BAA-6354AAF827C1}"/>
+    <hyperlink ref="A199" r:id="rId199" xr:uid="{026FD04C-DFFE-7446-BE19-7C692A5E7D45}"/>
+    <hyperlink ref="A200" r:id="rId200" xr:uid="{4B6827E9-5133-534F-A378-33B74C97B9E8}"/>
+    <hyperlink ref="A201" r:id="rId201" xr:uid="{905A9DFC-542E-3746-88AA-0613D26AEB4A}"/>
+    <hyperlink ref="A202" r:id="rId202" xr:uid="{6E0FAD1E-85C8-7E4D-999F-2443AC337F49}"/>
+    <hyperlink ref="A203" r:id="rId203" xr:uid="{94C5E53C-083C-8245-A3C0-DC78DF88F801}"/>
+    <hyperlink ref="A204" r:id="rId204" xr:uid="{C607D1D1-522F-A740-B5FE-C79E1B520964}"/>
+    <hyperlink ref="A205" r:id="rId205" xr:uid="{73B203FD-ABFE-004D-B61F-5481BBA0AB32}"/>
+    <hyperlink ref="A206" r:id="rId206" xr:uid="{8D2BC35C-0804-014C-8B5D-68D074DF97CE}"/>
+    <hyperlink ref="A207" r:id="rId207" xr:uid="{37880A7A-2513-6E44-BEC8-26F48632CFE2}"/>
+    <hyperlink ref="A208" r:id="rId208" xr:uid="{01CB8167-73D3-024D-97E8-7B9825772262}"/>
+    <hyperlink ref="A209" r:id="rId209" xr:uid="{D44C03AC-C3B4-3E4E-996A-AD53674D61AD}"/>
+    <hyperlink ref="A210" r:id="rId210" xr:uid="{25B5C679-739F-5242-B526-6BEA2ABCC9B4}"/>
+    <hyperlink ref="A211" r:id="rId211" xr:uid="{272862B1-AB15-064B-A4EF-D92DBCFFC594}"/>
+    <hyperlink ref="A212" r:id="rId212" xr:uid="{5E8D8D9E-D52D-354A-A4E9-227F493A2F3C}"/>
+    <hyperlink ref="A213" r:id="rId213" xr:uid="{43CD4AFC-0A4B-604A-9B63-432C8B184388}"/>
+    <hyperlink ref="A214" r:id="rId214" xr:uid="{C797B4FD-256C-7B47-8ABE-51742284D7C1}"/>
+    <hyperlink ref="A215" r:id="rId215" xr:uid="{9D43C380-B61B-0E45-9EFE-22F3D589228F}"/>
+    <hyperlink ref="A216" r:id="rId216" xr:uid="{5BF51224-D2D2-4E4F-94A8-0E264DBAE644}"/>
+    <hyperlink ref="A217" r:id="rId217" xr:uid="{0C5F26D2-9FCE-544D-BFCE-43E9E9B53798}"/>
+    <hyperlink ref="A218" r:id="rId218" xr:uid="{3DFD6606-C5E0-1947-A1B4-45FB0DDB2DEF}"/>
+    <hyperlink ref="A219" r:id="rId219" xr:uid="{008C6F3E-FC65-0C4C-A8E0-73CF59234684}"/>
+    <hyperlink ref="A220" r:id="rId220" xr:uid="{DF0FEFC5-427A-C047-ACD4-6C21318E1E23}"/>
+    <hyperlink ref="A221" r:id="rId221" xr:uid="{92AF8662-902C-804E-9030-0BAB9813C845}"/>
+    <hyperlink ref="A222" r:id="rId222" xr:uid="{71B613A7-0D55-7145-AC5B-02FD3BE2CAB8}"/>
+    <hyperlink ref="A223" r:id="rId223" xr:uid="{2CF44E20-9FFA-4B43-89C9-6E9FA6B19B52}"/>
+    <hyperlink ref="A224" r:id="rId224" xr:uid="{DB17333E-F6FC-FC49-B299-92058B80A305}"/>
+    <hyperlink ref="A225" r:id="rId225" xr:uid="{3CEFC6FF-932F-A24D-BF78-807549577A1C}"/>
+    <hyperlink ref="A226" r:id="rId226" xr:uid="{46BDDC05-1A90-B74E-A977-576480262C92}"/>
+    <hyperlink ref="A227" r:id="rId227" xr:uid="{738AEE97-2EE2-534E-8DDE-4341C066C6B6}"/>
+    <hyperlink ref="A228" r:id="rId228" xr:uid="{E7523842-A33A-DC45-8CCE-4066F5FB1B27}"/>
+    <hyperlink ref="A229" r:id="rId229" xr:uid="{79E590E7-0A9A-5841-9516-CCD47B597BF8}"/>
+    <hyperlink ref="A230" r:id="rId230" xr:uid="{7588C0D6-F57E-DD4E-AC90-724B07456150}"/>
+    <hyperlink ref="A231" r:id="rId231" xr:uid="{DE6D27E1-64D6-D842-AB75-774DE8229957}"/>
+    <hyperlink ref="A232" r:id="rId232" xr:uid="{01AF2C8D-352D-314A-8D6F-3B67A4C8C51E}"/>
+    <hyperlink ref="A233" r:id="rId233" xr:uid="{B117BD27-D7DB-7D45-9E62-17C0022E0C30}"/>
+    <hyperlink ref="A234" r:id="rId234" xr:uid="{7E805266-54F3-8D4B-96E6-DE90B976271C}"/>
+    <hyperlink ref="A235" r:id="rId235" xr:uid="{7FECA922-803E-B541-BD70-C92210259589}"/>
+    <hyperlink ref="A236" r:id="rId236" xr:uid="{A06C925D-130A-2C45-9FFA-E5ED62BCF903}"/>
+    <hyperlink ref="A237" r:id="rId237" xr:uid="{86952E20-34E4-BE4C-9B7E-05AE96D67C49}"/>
+    <hyperlink ref="A238" r:id="rId238" xr:uid="{428714E7-1F49-5E47-A7B4-FBB5FBE5B677}"/>
+    <hyperlink ref="A239" r:id="rId239" xr:uid="{CDCE6BC6-FEA9-E24F-97A1-BA6DAF9F3689}"/>
+    <hyperlink ref="A240" r:id="rId240" xr:uid="{9A51FAA8-CAF9-EB49-B871-9B7288385456}"/>
+    <hyperlink ref="A241" r:id="rId241" xr:uid="{5C9784D1-0EEF-5042-916F-E27F3BB19F64}"/>
+    <hyperlink ref="A242" r:id="rId242" xr:uid="{D4D8E38F-8C88-5A4F-8C1A-65B2122054A8}"/>
+    <hyperlink ref="A243" r:id="rId243" xr:uid="{921F652B-C654-EE43-928D-3E9B698DE534}"/>
+    <hyperlink ref="A244" r:id="rId244" xr:uid="{DE0AAE01-548C-7A4E-8C00-7F53FFB019F1}"/>
+    <hyperlink ref="A245" r:id="rId245" xr:uid="{66321B79-3291-6744-B4F3-AA7875F908CD}"/>
+    <hyperlink ref="A246" r:id="rId246" xr:uid="{C1F12D44-80AA-2B4A-9918-ABD7B564E6D1}"/>
+    <hyperlink ref="A247" r:id="rId247" xr:uid="{CFBA8119-5235-3547-A11B-DE68DC150A56}"/>
+    <hyperlink ref="A248" r:id="rId248" xr:uid="{6586FC0D-D311-8F47-A84E-82044CA7AF00}"/>
+    <hyperlink ref="A249" r:id="rId249" xr:uid="{5168A552-E3CB-AC40-AB67-25F57D51FADC}"/>
+    <hyperlink ref="A250" r:id="rId250" xr:uid="{5EFEAE08-0D33-3540-A0B7-4080163E0257}"/>
+    <hyperlink ref="A251" r:id="rId251" xr:uid="{8B9E93C8-0330-9944-9569-068E818AC275}"/>
+    <hyperlink ref="A252" r:id="rId252" xr:uid="{8FE95D37-BEBC-F645-8547-C28857B0A45C}"/>
+    <hyperlink ref="A253" r:id="rId253" xr:uid="{D89CCFEC-D0A3-8B48-8AD9-B1DBBC58B978}"/>
+    <hyperlink ref="A254" r:id="rId254" xr:uid="{8EFFFD9C-30C7-4048-9576-B9744E0AAA6D}"/>
+    <hyperlink ref="A255" r:id="rId255" xr:uid="{6A1239DA-4F6F-324B-8406-E5968BF79193}"/>
+    <hyperlink ref="A256" r:id="rId256" xr:uid="{1FB0358F-8137-E346-8B37-A88DA58FF893}"/>
+    <hyperlink ref="A257" r:id="rId257" xr:uid="{7393D797-F331-2747-B21F-9C64477B03E8}"/>
+    <hyperlink ref="A258" r:id="rId258" xr:uid="{89241C78-8C33-8A4B-9191-27ABCFD624DD}"/>
+    <hyperlink ref="A259" r:id="rId259" xr:uid="{58611FFD-E629-A44B-8459-DBE392F39DDE}"/>
+    <hyperlink ref="A260" r:id="rId260" xr:uid="{FC27C60A-E408-804E-855C-1CBA151805E0}"/>
+    <hyperlink ref="A261" r:id="rId261" xr:uid="{31CA7AA2-EF5D-DA44-B167-D56CD35E223C}"/>
+    <hyperlink ref="A262" r:id="rId262" xr:uid="{DDC1BD5A-FC66-FB42-B1CB-034865EC2803}"/>
+    <hyperlink ref="A263" r:id="rId263" xr:uid="{8BD644BD-BAF3-7544-860E-00515810E7AE}"/>
+    <hyperlink ref="A264" r:id="rId264" xr:uid="{55FC32CC-5C56-4E43-99E9-7FCFD2E9E866}"/>
+    <hyperlink ref="A265" r:id="rId265" xr:uid="{9F390145-95BE-1D41-8C2C-241EBBE828EF}"/>
+    <hyperlink ref="A266" r:id="rId266" xr:uid="{05530643-B829-EE42-81CA-23F84CE6A2EF}"/>
+    <hyperlink ref="A267" r:id="rId267" xr:uid="{28D44972-71E5-D642-A427-2F69E1E61BB5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>

</xml_diff>